<commit_message>
Corrected parentheses in all scripts
</commit_message>
<xml_diff>
--- a/specifications/5_Insects/ScriptRules_Insects.xlsx
+++ b/specifications/5_Insects/ScriptRules_Insects.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\HgRepos\landfiredisturbance\specifications\5_Insects\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\HgRepos\LANDFIRE\landfiredisturbance-clone\specifications\5_Insects\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -1180,12 +1180,6 @@
     <t>* = 2</t>
   </si>
   <si>
-    <t>* = (1/1.5)</t>
-  </si>
-  <si>
-    <t>* = (1/2)</t>
-  </si>
-  <si>
     <t>* = 1.25, min = 4</t>
   </si>
   <si>
@@ -1721,6 +1715,12 @@
   </si>
   <si>
     <t>* = 0.75</t>
+  </si>
+  <si>
+    <t>* = 1/1.5</t>
+  </si>
+  <si>
+    <t>* = 1/2</t>
   </si>
 </sst>
 </file>
@@ -2923,23 +2923,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K952"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="A34" sqref="A34"/>
+    <sheetView tabSelected="1" topLeftCell="A45" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="K107" sqref="K107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="74" style="37" customWidth="1"/>
     <col min="2" max="2" width="28" customWidth="1"/>
-    <col min="3" max="3" width="48.5703125" style="31" customWidth="1"/>
-    <col min="4" max="4" width="50.7109375" style="35" customWidth="1"/>
-    <col min="5" max="5" width="28.7109375" style="36" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="48.5703125" style="31" customWidth="1"/>
-    <col min="7" max="7" width="48.5703125" style="35" customWidth="1"/>
-    <col min="8" max="8" width="20.28515625" style="36" customWidth="1"/>
-    <col min="9" max="9" width="50.7109375" style="31" customWidth="1"/>
-    <col min="10" max="10" width="48.5703125" style="35" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="20.28515625" style="36" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.7109375" style="31" customWidth="1"/>
+    <col min="4" max="4" width="19.7109375" style="35" customWidth="1"/>
+    <col min="5" max="5" width="19.7109375" style="36" customWidth="1"/>
+    <col min="6" max="6" width="19.7109375" style="31" customWidth="1"/>
+    <col min="7" max="7" width="19.7109375" style="35" customWidth="1"/>
+    <col min="8" max="8" width="19.7109375" style="36" customWidth="1"/>
+    <col min="9" max="9" width="19.7109375" style="31" customWidth="1"/>
+    <col min="10" max="10" width="19.7109375" style="35" customWidth="1"/>
+    <col min="11" max="11" width="19.7109375" style="36" customWidth="1"/>
     <col min="12" max="16384" width="9.140625" style="37"/>
   </cols>
   <sheetData>
@@ -2963,7 +2963,7 @@
     </row>
     <row r="2" spans="1:11" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="C2" s="31" t="s">
         <v>15</v>
@@ -2998,7 +2998,7 @@
         <v>98</v>
       </c>
       <c r="B3" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="C3" s="31" t="s">
         <v>0</v>
@@ -3024,7 +3024,7 @@
         <v>93</v>
       </c>
       <c r="B4" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -3032,13 +3032,13 @@
         <v>95</v>
       </c>
       <c r="B5" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="C5" s="31" t="s">
         <v>1</v>
       </c>
       <c r="D5" s="32" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="F5" s="31" t="s">
         <v>13</v>
@@ -3052,7 +3052,7 @@
         <v>94</v>
       </c>
       <c r="B6" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
@@ -3060,7 +3060,7 @@
         <v>96</v>
       </c>
       <c r="B7" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="C7" s="31" t="s">
         <v>0</v>
@@ -3086,7 +3086,7 @@
         <v>97</v>
       </c>
       <c r="B8" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="C8" s="31" t="s">
         <v>0</v>
@@ -3112,7 +3112,7 @@
         <v>88</v>
       </c>
       <c r="B9" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
@@ -3120,13 +3120,13 @@
         <v>90</v>
       </c>
       <c r="B10" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="C10" s="31" t="s">
         <v>1</v>
       </c>
       <c r="D10" s="32" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="F10" s="31" t="s">
         <v>13</v>
@@ -3140,7 +3140,7 @@
         <v>89</v>
       </c>
       <c r="B11" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
@@ -3148,7 +3148,7 @@
         <v>91</v>
       </c>
       <c r="B12" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="C12" s="31" t="s">
         <v>0</v>
@@ -3174,7 +3174,7 @@
         <v>92</v>
       </c>
       <c r="B13" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="C13" s="31" t="s">
         <v>0</v>
@@ -3200,7 +3200,7 @@
         <v>99</v>
       </c>
       <c r="B14" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
@@ -3208,7 +3208,7 @@
         <v>101</v>
       </c>
       <c r="B15" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
@@ -3216,7 +3216,7 @@
         <v>100</v>
       </c>
       <c r="B16" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
@@ -3224,7 +3224,7 @@
         <v>102</v>
       </c>
       <c r="B17" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
@@ -3232,7 +3232,7 @@
         <v>103</v>
       </c>
       <c r="B18" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
@@ -3240,25 +3240,25 @@
         <v>74</v>
       </c>
       <c r="B19" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="D19" s="32" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="E19" s="44" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="G19" s="32" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="H19" s="44" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="J19" s="32" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="K19" s="44" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
@@ -3266,25 +3266,25 @@
         <v>75</v>
       </c>
       <c r="B20" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="D20" s="32" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="E20" s="44" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="G20" s="32" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="H20" s="44" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="J20" s="32" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="K20" s="44" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
@@ -3292,25 +3292,25 @@
         <v>76</v>
       </c>
       <c r="B21" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="D21" s="32" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="E21" s="44" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="G21" s="32" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="H21" s="44" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="J21" s="32" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="K21" s="44" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
@@ -3318,26 +3318,26 @@
         <v>79</v>
       </c>
       <c r="B22" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="C22" s="31" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="D22" s="43" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="E22" s="33"/>
       <c r="F22" s="31" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="G22" s="43" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="I22" s="31" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="J22" s="43" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
@@ -3345,26 +3345,26 @@
         <v>77</v>
       </c>
       <c r="B23" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="C23" s="31" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="D23" s="43" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="E23" s="33"/>
       <c r="F23" s="31" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="G23" s="43" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="I23" s="31" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="J23" s="43" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
@@ -3372,26 +3372,26 @@
         <v>78</v>
       </c>
       <c r="B24" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="C24" s="31" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="D24" s="43" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="E24" s="33"/>
       <c r="F24" s="31" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="G24" s="43" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="I24" s="31" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="J24" s="43" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
@@ -3399,26 +3399,26 @@
         <v>80</v>
       </c>
       <c r="B25" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="C25" s="31" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="D25" s="43" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="E25" s="33"/>
       <c r="F25" s="45" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="G25" s="43" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="I25" s="45" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="J25" s="43" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
@@ -3426,34 +3426,34 @@
         <v>81</v>
       </c>
       <c r="B26" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="C26" s="31" t="s">
+        <v>390</v>
+      </c>
+      <c r="D26" s="43" t="s">
+        <v>391</v>
+      </c>
+      <c r="E26" s="33" t="s">
+        <v>379</v>
+      </c>
+      <c r="F26" s="31" t="s">
         <v>392</v>
       </c>
-      <c r="D26" s="43" t="s">
-        <v>393</v>
-      </c>
-      <c r="E26" s="33" t="s">
-        <v>381</v>
-      </c>
-      <c r="F26" s="31" t="s">
+      <c r="G26" s="43" t="s">
+        <v>390</v>
+      </c>
+      <c r="H26" s="33" t="s">
+        <v>379</v>
+      </c>
+      <c r="I26" s="31" t="s">
         <v>394</v>
       </c>
-      <c r="G26" s="43" t="s">
-        <v>392</v>
-      </c>
-      <c r="H26" s="33" t="s">
-        <v>381</v>
-      </c>
-      <c r="I26" s="31" t="s">
-        <v>396</v>
-      </c>
       <c r="J26" s="43" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="K26" s="33" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
@@ -3461,25 +3461,25 @@
         <v>82</v>
       </c>
       <c r="B27" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="D27" s="32" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="E27" s="44" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="G27" s="32" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="H27" s="44" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="J27" s="32" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="K27" s="44" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
@@ -3487,25 +3487,25 @@
         <v>83</v>
       </c>
       <c r="B28" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="D28" s="32" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="E28" s="44" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="G28" s="32" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="H28" s="44" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="J28" s="32" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="K28" s="44" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
@@ -3513,25 +3513,25 @@
         <v>84</v>
       </c>
       <c r="B29" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="D29" s="32" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="E29" s="44" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="G29" s="32" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="H29" s="44" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="J29" s="32" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="K29" s="44" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
@@ -3539,25 +3539,25 @@
         <v>85</v>
       </c>
       <c r="B30" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="D30" s="32" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="E30" s="44" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="G30" s="32" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="H30" s="44" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="J30" s="32" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="K30" s="44" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
@@ -3565,25 +3565,25 @@
         <v>86</v>
       </c>
       <c r="B31" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="D31" s="32" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="E31" s="44" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="G31" s="32" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="H31" s="44" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="J31" s="32" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="K31" s="44" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
@@ -3591,25 +3591,25 @@
         <v>87</v>
       </c>
       <c r="B32" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="D32" s="32" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="E32" s="44" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="G32" s="32" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="H32" s="44" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="J32" s="32" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="K32" s="44" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
@@ -3617,7 +3617,7 @@
         <v>72</v>
       </c>
       <c r="B33" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
@@ -3625,7 +3625,7 @@
         <v>73</v>
       </c>
       <c r="B34" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
@@ -3633,7 +3633,7 @@
         <v>138</v>
       </c>
       <c r="B35" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="E35" s="33"/>
       <c r="J35" s="32"/>
@@ -3644,7 +3644,7 @@
         <v>139</v>
       </c>
       <c r="B36" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="E36" s="33"/>
       <c r="J36" s="32" t="s">
@@ -3657,7 +3657,7 @@
         <v>140</v>
       </c>
       <c r="B37" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="E37" s="33"/>
       <c r="J37" s="32"/>
@@ -3668,7 +3668,7 @@
         <v>141</v>
       </c>
       <c r="B38" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="E38" s="33"/>
       <c r="J38" s="32"/>
@@ -3679,7 +3679,7 @@
         <v>142</v>
       </c>
       <c r="B39" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="E39" s="33"/>
       <c r="J39" s="32" t="s">
@@ -3692,7 +3692,7 @@
         <v>143</v>
       </c>
       <c r="B40" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="E40" s="33"/>
       <c r="J40" s="32"/>
@@ -3703,7 +3703,7 @@
         <v>116</v>
       </c>
       <c r="B41" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="D41" s="32"/>
       <c r="G41" s="32"/>
@@ -3715,7 +3715,7 @@
         <v>117</v>
       </c>
       <c r="B42" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="D42" s="32"/>
       <c r="G42" s="35" t="s">
@@ -3731,7 +3731,7 @@
         <v>118</v>
       </c>
       <c r="B43" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="D43" s="32"/>
       <c r="G43" s="35" t="s">
@@ -3747,7 +3747,7 @@
         <v>119</v>
       </c>
       <c r="B44" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="D44" s="32"/>
       <c r="G44" s="32"/>
@@ -3759,7 +3759,7 @@
         <v>120</v>
       </c>
       <c r="B45" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="D45" s="32"/>
       <c r="J45" s="32"/>
@@ -3770,7 +3770,7 @@
         <v>121</v>
       </c>
       <c r="B46" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="D46" s="32"/>
       <c r="G46" s="35" t="s">
@@ -3786,7 +3786,7 @@
         <v>122</v>
       </c>
       <c r="B47" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="D47" s="32"/>
       <c r="G47" s="35" t="s">
@@ -3802,7 +3802,7 @@
         <v>123</v>
       </c>
       <c r="B48" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="D48" s="32"/>
       <c r="G48" s="32"/>
@@ -3814,7 +3814,7 @@
         <v>144</v>
       </c>
       <c r="B49" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="D49" s="32" t="s">
         <v>1</v>
@@ -3838,7 +3838,7 @@
         <v>145</v>
       </c>
       <c r="B50" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="D50" s="32" t="s">
         <v>1</v>
@@ -3862,7 +3862,7 @@
         <v>149</v>
       </c>
       <c r="B51" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="D51" s="32" t="s">
         <v>1</v>
@@ -3877,10 +3877,10 @@
         <v>225</v>
       </c>
       <c r="J51" s="32" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="K51" s="33" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.25">
@@ -3888,7 +3888,7 @@
         <v>150</v>
       </c>
       <c r="B52" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="D52" s="32" t="s">
         <v>1</v>
@@ -3903,10 +3903,10 @@
         <v>224</v>
       </c>
       <c r="J52" s="32" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="K52" s="33" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.25">
@@ -3914,7 +3914,7 @@
         <v>151</v>
       </c>
       <c r="B53" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="D53" s="32" t="s">
         <v>1</v>
@@ -3929,10 +3929,10 @@
         <v>223</v>
       </c>
       <c r="J53" s="32" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="K53" s="33" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.25">
@@ -3940,17 +3940,17 @@
         <v>193</v>
       </c>
       <c r="B54" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="E54" s="33" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="G54" s="46"/>
       <c r="H54" s="36" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="K54" s="36" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.25">
@@ -3958,17 +3958,17 @@
         <v>194</v>
       </c>
       <c r="B55" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="E55" s="33" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="G55" s="46"/>
       <c r="H55" s="36" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="K55" s="36" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.25">
@@ -3976,17 +3976,17 @@
         <v>195</v>
       </c>
       <c r="B56" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="E56" s="33" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="G56" s="46"/>
       <c r="H56" s="36" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="K56" s="36" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.25">
@@ -3994,16 +3994,16 @@
         <v>196</v>
       </c>
       <c r="B57" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="E57" s="33" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="H57" s="33" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="K57" s="33" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.25">
@@ -4011,16 +4011,16 @@
         <v>197</v>
       </c>
       <c r="B58" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="E58" s="33" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="H58" s="33" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="K58" s="33" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.25">
@@ -4028,16 +4028,16 @@
         <v>198</v>
       </c>
       <c r="B59" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="E59" s="33" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="H59" s="33" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="K59" s="33" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.25">
@@ -4045,7 +4045,7 @@
         <v>158</v>
       </c>
       <c r="B60" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.25">
@@ -4053,7 +4053,7 @@
         <v>159</v>
       </c>
       <c r="B61" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.25">
@@ -4061,7 +4061,7 @@
         <v>160</v>
       </c>
       <c r="B62" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.25">
@@ -4069,7 +4069,7 @@
         <v>155</v>
       </c>
       <c r="B63" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.25">
@@ -4077,7 +4077,7 @@
         <v>156</v>
       </c>
       <c r="B64" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.25">
@@ -4085,7 +4085,7 @@
         <v>157</v>
       </c>
       <c r="B65" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.25">
@@ -4093,7 +4093,7 @@
         <v>152</v>
       </c>
       <c r="B66" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.25">
@@ -4101,7 +4101,7 @@
         <v>153</v>
       </c>
       <c r="B67" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.25">
@@ -4109,7 +4109,7 @@
         <v>154</v>
       </c>
       <c r="B68" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.25">
@@ -4117,7 +4117,7 @@
         <v>146</v>
       </c>
       <c r="B69" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
     </row>
     <row r="70" spans="1:10" x14ac:dyDescent="0.25">
@@ -4125,7 +4125,7 @@
         <v>147</v>
       </c>
       <c r="B70" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
     </row>
     <row r="71" spans="1:10" x14ac:dyDescent="0.25">
@@ -4133,7 +4133,7 @@
         <v>148</v>
       </c>
       <c r="B71" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
     </row>
     <row r="72" spans="1:10" x14ac:dyDescent="0.25">
@@ -4141,7 +4141,7 @@
         <v>124</v>
       </c>
       <c r="B72" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
     </row>
     <row r="73" spans="1:10" x14ac:dyDescent="0.25">
@@ -4149,7 +4149,7 @@
         <v>125</v>
       </c>
       <c r="B73" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
     </row>
     <row r="74" spans="1:10" x14ac:dyDescent="0.25">
@@ -4157,7 +4157,7 @@
         <v>126</v>
       </c>
       <c r="B74" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
     </row>
     <row r="75" spans="1:10" x14ac:dyDescent="0.25">
@@ -4165,7 +4165,7 @@
         <v>127</v>
       </c>
       <c r="B75" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
     </row>
     <row r="76" spans="1:10" x14ac:dyDescent="0.25">
@@ -4173,7 +4173,7 @@
         <v>128</v>
       </c>
       <c r="B76" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
     </row>
     <row r="77" spans="1:10" x14ac:dyDescent="0.25">
@@ -4181,7 +4181,7 @@
         <v>129</v>
       </c>
       <c r="B77" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
     </row>
     <row r="78" spans="1:10" x14ac:dyDescent="0.25">
@@ -4189,7 +4189,7 @@
         <v>130</v>
       </c>
       <c r="B78" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
     </row>
     <row r="79" spans="1:10" x14ac:dyDescent="0.25">
@@ -4197,7 +4197,7 @@
         <v>131</v>
       </c>
       <c r="B79" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="D79" s="32"/>
       <c r="J79" s="32"/>
@@ -4207,7 +4207,7 @@
         <v>132</v>
       </c>
       <c r="B80" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="D80" s="32"/>
       <c r="J80" s="32"/>
@@ -4217,25 +4217,25 @@
         <v>133</v>
       </c>
       <c r="B81" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="D81" s="32" t="s">
         <v>1</v>
       </c>
       <c r="E81" s="33" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="G81" s="35" t="s">
         <v>14</v>
       </c>
       <c r="H81" s="33" t="s">
-        <v>228</v>
+        <v>407</v>
       </c>
       <c r="J81" s="32" t="s">
         <v>227</v>
       </c>
       <c r="K81" s="33" t="s">
-        <v>229</v>
+        <v>408</v>
       </c>
     </row>
     <row r="82" spans="1:11" x14ac:dyDescent="0.25">
@@ -4243,25 +4243,25 @@
         <v>134</v>
       </c>
       <c r="B82" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="D82" s="32" t="s">
         <v>1</v>
       </c>
       <c r="E82" s="33" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="G82" s="35" t="s">
         <v>14</v>
       </c>
       <c r="H82" s="33" t="s">
-        <v>228</v>
+        <v>407</v>
       </c>
       <c r="J82" s="32" t="s">
         <v>227</v>
       </c>
       <c r="K82" s="33" t="s">
-        <v>229</v>
+        <v>408</v>
       </c>
     </row>
     <row r="83" spans="1:11" x14ac:dyDescent="0.25">
@@ -4269,7 +4269,7 @@
         <v>135</v>
       </c>
       <c r="B83" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="D83" s="32"/>
       <c r="J83" s="32"/>
@@ -4279,7 +4279,7 @@
         <v>136</v>
       </c>
       <c r="B84" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="D84" s="32"/>
       <c r="J84" s="32"/>
@@ -4289,7 +4289,7 @@
         <v>109</v>
       </c>
       <c r="B85" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="D85" s="32"/>
     </row>
@@ -4298,7 +4298,7 @@
         <v>110</v>
       </c>
       <c r="B86" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="D86" s="32"/>
     </row>
@@ -4307,7 +4307,7 @@
         <v>111</v>
       </c>
       <c r="B87" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="D87" s="32"/>
       <c r="E87" s="33"/>
@@ -4323,7 +4323,7 @@
         <v>112</v>
       </c>
       <c r="B88" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="D88" s="32"/>
       <c r="H88" s="33" t="s">
@@ -4338,7 +4338,7 @@
         <v>106</v>
       </c>
       <c r="B89" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="D89" s="32"/>
     </row>
@@ -4347,7 +4347,7 @@
         <v>107</v>
       </c>
       <c r="B90" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="D90" s="32"/>
     </row>
@@ -4356,7 +4356,7 @@
         <v>108</v>
       </c>
       <c r="B91" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="D91" s="32"/>
     </row>
@@ -4365,7 +4365,7 @@
         <v>113</v>
       </c>
       <c r="B92" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="D92" s="32"/>
     </row>
@@ -4374,7 +4374,7 @@
         <v>114</v>
       </c>
       <c r="B93" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="D93" s="32"/>
     </row>
@@ -4383,7 +4383,7 @@
         <v>115</v>
       </c>
       <c r="B94" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="D94" s="32"/>
     </row>
@@ -7736,7 +7736,7 @@
         <v>33</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="C1" s="38" t="s">
         <v>212</v>
@@ -7826,7 +7826,7 @@
         <v>eCANOPY_TREES_TOTAL_PERCENT_COVER</v>
       </c>
       <c r="B2" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="C2" s="5">
         <v>0.9</v>
@@ -7926,7 +7926,7 @@
         <v>eCANOPY_TREES_OVERSTORY_DIAMETER_AT_BREAST_HEIGHT</v>
       </c>
       <c r="B3" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="C3" s="5"/>
       <c r="D3" s="6"/>
@@ -8022,7 +8022,7 @@
         <v>eCANOPY_TREES_OVERSTORY_HEIGHT_TO_LIVE_CROWN</v>
       </c>
       <c r="B4" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="C4" s="5">
         <v>1.1000000000000001</v>
@@ -8122,7 +8122,7 @@
         <v>eCANOPY_TREES_OVERSTORY_HEIGHT</v>
       </c>
       <c r="B5" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="C5" s="5"/>
       <c r="D5" s="6"/>
@@ -8218,7 +8218,7 @@
         <v>eCANOPY_TREES_OVERSTORY_PERCENT_COVER</v>
       </c>
       <c r="B6" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="C6" s="5">
         <v>0.9</v>
@@ -8318,7 +8318,7 @@
         <v>eCANOPY_TREES_OVERSTORY_STEM_DENSITY</v>
       </c>
       <c r="B7" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="C7" s="5">
         <v>0.9</v>
@@ -8418,7 +8418,7 @@
         <v>eCANOPY_TREES_MIDSTORY_DIAMETER_AT_BREAST_HEIGHT</v>
       </c>
       <c r="B8" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="C8" s="5"/>
       <c r="D8" s="6"/>
@@ -8505,7 +8505,7 @@
         <v>eCANOPY_TREES_MIDSTORY_HEIGHT_TO_LIVE_CROWN</v>
       </c>
       <c r="B9" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="C9" s="5">
         <v>1.1000000000000001</v>
@@ -8596,7 +8596,7 @@
         <v>eCANOPY_TREES_MIDSTORY_HEIGHT</v>
       </c>
       <c r="B10" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="C10" s="5"/>
       <c r="D10" s="6"/>
@@ -8683,7 +8683,7 @@
         <v>eCANOPY_TREES_MIDSTORY_PERCENT_COVER</v>
       </c>
       <c r="B11" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="C11" s="5">
         <v>0.9</v>
@@ -8774,7 +8774,7 @@
         <v>eCANOPY_TREES_MIDSTORY_STEM_DENSITY</v>
       </c>
       <c r="B12" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="C12" s="5">
         <v>0.9</v>
@@ -8865,7 +8865,7 @@
         <v>eCANOPY_TREES_UNDERSTORY_DIAMETER_AT_BREAST_HEIGHT</v>
       </c>
       <c r="B13" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="C13" s="5"/>
       <c r="D13" s="6"/>
@@ -8958,7 +8958,7 @@
         <v>eCANOPY_TREES_UNDERSTORY_HEIGHT_TO_LIVE_CROWN</v>
       </c>
       <c r="B14" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="C14" s="5"/>
       <c r="D14" s="6"/>
@@ -9051,7 +9051,7 @@
         <v>eCANOPY_TREES_UNDERSTORY_HEIGHT</v>
       </c>
       <c r="B15" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="C15" s="5"/>
       <c r="D15" s="6"/>
@@ -9144,7 +9144,7 @@
         <v>eCANOPY_TREES_UNDERSTORY_PERCENT_COVER</v>
       </c>
       <c r="B16" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="C16" s="5"/>
       <c r="D16" s="6"/>
@@ -9237,7 +9237,7 @@
         <v>eCANOPY_TREES_UNDERSTORY_STEM_DENSITY</v>
       </c>
       <c r="B17" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="C17" s="5"/>
       <c r="D17" s="6"/>
@@ -9330,14 +9330,14 @@
         <v>eCANOPY_SNAGS_CLASS_1_ALL_OTHERS_DIAMETER</v>
       </c>
       <c r="B18" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="C18" s="47"/>
       <c r="D18" s="49" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="E18" s="50" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="G18" s="14">
         <f>F18</f>
@@ -9424,14 +9424,14 @@
         <v>eCANOPY_SNAGS_CLASS_1_ALL_OTHERS_HEIGHT</v>
       </c>
       <c r="B19" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="C19" s="47"/>
       <c r="D19" s="49" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="E19" s="50" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="G19" s="14">
         <f>F19</f>
@@ -9518,14 +9518,14 @@
         <v>eCANOPY_SNAGS_CLASS_1_ALL_OTHERS_STEM_DENSITY</v>
       </c>
       <c r="B20" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="C20" s="53"/>
       <c r="D20" s="49" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="E20" s="50" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="G20" s="14">
         <f>F20</f>
@@ -9612,13 +9612,13 @@
         <v>eCANOPY_SNAGS_CLASS_1_CONIFERS_WITH_FOLIAGE_HEIGHT_TO_CROWN_BASE</v>
       </c>
       <c r="B21" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="C21" s="55" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="D21" s="51" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="E21" s="41">
         <v>0</v>
@@ -9705,13 +9705,13 @@
         <v>eCANOPY_SNAGS_CLASS_1_CONIFERS_WITH_FOLIAGE_DIAMETER</v>
       </c>
       <c r="B22" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="C22" s="55" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="D22" s="51" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="E22" s="41">
         <v>0</v>
@@ -9798,13 +9798,13 @@
         <v>eCANOPY_SNAGS_CLASS_1_CONIFERS_WITH_FOLIAGE_HEIGHT</v>
       </c>
       <c r="B23" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="C23" s="55" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="D23" s="51" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="E23" s="41">
         <v>0</v>
@@ -9891,13 +9891,13 @@
         <v>eCANOPY_SNAGS_CLASS_1_CONIFERS_WITH_FOLIAGE_PERCENT_COVER</v>
       </c>
       <c r="B24" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="C24" s="55" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="D24" s="51" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="E24" s="41">
         <v>0</v>
@@ -9984,13 +9984,13 @@
         <v>eCANOPY_SNAGS_CLASS_1_CONIFERS_WITH_FOLIAGE_STEM_DENSITY</v>
       </c>
       <c r="B25" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="C25" s="55" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="D25" s="51" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="E25" s="41">
         <v>0</v>
@@ -10077,14 +10077,14 @@
         <v>eCANOPY_SNAGS_CLASS_2_DIAMETER</v>
       </c>
       <c r="B26" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="C26" s="55"/>
       <c r="D26" s="49" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="E26" s="50" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="G26" s="14">
         <f t="shared" ref="G26:G33" si="54">F26</f>
@@ -10174,14 +10174,14 @@
         <v>eCANOPY_SNAGS_CLASS_2_HEIGHT</v>
       </c>
       <c r="B27" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="C27" s="54"/>
       <c r="D27" s="49" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="E27" s="50" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="G27" s="14">
         <f t="shared" si="54"/>
@@ -10271,14 +10271,14 @@
         <v>eCANOPY_SNAGS_CLASS_2_STEM_DENSITY</v>
       </c>
       <c r="B28" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="C28" s="47"/>
       <c r="D28" s="49" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="E28" s="50" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="G28" s="14">
         <f t="shared" si="54"/>
@@ -10368,14 +10368,14 @@
         <v>eCANOPY_SNAGS_CLASS_3_DIAMETER</v>
       </c>
       <c r="B29" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="C29" s="47"/>
       <c r="D29" s="49" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="E29" s="50" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="F29" s="13">
         <v>9</v>
@@ -10468,14 +10468,14 @@
         <v>eCANOPY_SNAGS_CLASS_3_HEIGHT</v>
       </c>
       <c r="B30" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="C30" s="47"/>
       <c r="D30" s="49" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="E30" s="50" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="F30" s="13">
         <v>60</v>
@@ -10568,14 +10568,14 @@
         <v>eCANOPY_SNAGS_CLASS_3_STEM_DENSITY</v>
       </c>
       <c r="B31" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="C31" s="47"/>
       <c r="D31" s="49" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="E31" s="50" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="F31" s="13">
         <v>3</v>
@@ -10668,7 +10668,7 @@
         <v>eCANOPY_LADDER_FUELS_MAXIMUM_HEIGHT</v>
       </c>
       <c r="B32" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="C32" s="5"/>
       <c r="D32" s="6"/>
@@ -10758,7 +10758,7 @@
         <v>eCANOPY_LADDER_FUELS_MINIMUM_HEIGHT</v>
       </c>
       <c r="B33" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="C33" s="5"/>
       <c r="D33" s="6"/>
@@ -10848,7 +10848,7 @@
         <v>eSHRUBS_PRIMARY_LAYER_HEIGHT</v>
       </c>
       <c r="B34" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="C34" s="5"/>
       <c r="D34" s="6"/>
@@ -10950,7 +10950,7 @@
         <v>eSHRUBS_PRIMARY_LAYER_PERCENT_COVER</v>
       </c>
       <c r="B35" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="C35" s="5"/>
       <c r="D35" s="6"/>
@@ -11052,7 +11052,7 @@
         <v>eSHRUBS_PRIMARY_LAYER_PERCENT_LIVE</v>
       </c>
       <c r="B36" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="C36" s="5"/>
       <c r="D36" s="6"/>
@@ -11154,7 +11154,7 @@
         <v>eSHRUBS_SECONDARY_LAYER_HEIGHT</v>
       </c>
       <c r="B37" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="C37" s="5"/>
       <c r="D37" s="6"/>
@@ -11247,7 +11247,7 @@
         <v>eSHRUBS_SECONDARY_LAYER_PERCENT_COVER</v>
       </c>
       <c r="B38" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="C38" s="5"/>
       <c r="D38" s="6"/>
@@ -11340,7 +11340,7 @@
         <v>eSHRUBS_SECONDARY_LAYER_PERCENT_LIVE</v>
       </c>
       <c r="B39" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="C39" s="5"/>
       <c r="D39" s="6"/>
@@ -11433,7 +11433,7 @@
         <v>eHERBACEOUS_PRIMARY_LAYER_HEIGHT</v>
       </c>
       <c r="B40" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="C40" s="5"/>
       <c r="D40" s="6"/>
@@ -11532,7 +11532,7 @@
         <v>eHERBACEOUS_PRIMARY_LAYER_LOADING</v>
       </c>
       <c r="B41" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="C41" s="5"/>
       <c r="D41" s="6"/>
@@ -11631,7 +11631,7 @@
         <v>eHERBACEOUS_PRIMARY_LAYER_PERCENT_COVER</v>
       </c>
       <c r="B42" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="C42" s="5"/>
       <c r="D42" s="6"/>
@@ -11730,7 +11730,7 @@
         <v>eHERBACEOUS_PRIMARY_LAYER_PERCENT_LIVE</v>
       </c>
       <c r="B43" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="C43" s="5"/>
       <c r="D43" s="6"/>
@@ -11829,7 +11829,7 @@
         <v>eHERBACEOUS_SECONDARY_LAYER_HEIGHT</v>
       </c>
       <c r="B44" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C44" s="5"/>
       <c r="D44" s="6"/>
@@ -11925,7 +11925,7 @@
         <v>eHERBACEOUS_SECONDARY_LAYER_LOADING</v>
       </c>
       <c r="B45" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="C45" s="5"/>
       <c r="D45" s="6"/>
@@ -12021,7 +12021,7 @@
         <v>eHERBACEOUS_SECONDARY_LAYER_PERCENT_COVER</v>
       </c>
       <c r="B46" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="C46" s="5"/>
       <c r="D46" s="6"/>
@@ -12117,7 +12117,7 @@
         <v>eHERBACEOUS_SECONDARY_LAYER_PERCENT_LIVE</v>
       </c>
       <c r="B47" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="C47" s="5"/>
       <c r="D47" s="6"/>
@@ -12213,7 +12213,7 @@
         <v>eWOODY_FUEL_ALL_DOWNED_WOODY_FUEL_DEPTH</v>
       </c>
       <c r="B48" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="C48" s="5"/>
       <c r="D48" s="6">
@@ -12316,7 +12316,7 @@
         <v>eWOODY_FUEL_ALL_DOWNED_WOODY_FUEL_TOTAL_PERCENT_COVER</v>
       </c>
       <c r="B49" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="C49" s="5"/>
       <c r="D49" s="6">
@@ -12419,7 +12419,7 @@
         <v>eWOODY_FUEL_SOUND_WOOD_LOADINGS_ZERO_TO_THREE_INCHES_ONE_TO_THREE_INCHES</v>
       </c>
       <c r="B50" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="C50" s="5"/>
       <c r="D50" s="6">
@@ -12522,7 +12522,7 @@
         <v>eWOODY_FUEL_SOUND_WOOD_LOADINGS_ZERO_TO_THREE_INCHES_QUARTER_INCH_TO_ONE_INCH</v>
       </c>
       <c r="B51" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="C51" s="5"/>
       <c r="D51" s="6">
@@ -12625,7 +12625,7 @@
         <v>eWOODY_FUEL_SOUND_WOOD_LOADINGS_ZERO_TO_THREE_INCHES_ZERO_TO_QUARTER_INCH</v>
       </c>
       <c r="B52" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="C52" s="5"/>
       <c r="D52" s="6">
@@ -12728,7 +12728,7 @@
         <v>eWOODY_FUEL_SOUND_WOOD_LOADINGS_GREATER_THAN_THREE_INCHES_THREE_TO_NINE_INCHES</v>
       </c>
       <c r="B53" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="C53" s="5"/>
       <c r="D53" s="6"/>
@@ -12829,7 +12829,7 @@
         <v>eWOODY_FUEL_SOUND_WOOD_LOADINGS_GREATER_THAN_THREE_INCHES_NINE_TO_TWENTY_INCHES</v>
       </c>
       <c r="B54" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="C54" s="5"/>
       <c r="D54" s="6"/>
@@ -12930,7 +12930,7 @@
         <v>eWOODY_FUEL_SOUND_WOOD_LOADINGS_GREATER_THAN_THREE_INCHES_GREATER_THAN_TWENTY_INCHES</v>
       </c>
       <c r="B55" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="C55" s="5"/>
       <c r="D55" s="6"/>
@@ -13031,12 +13031,12 @@
         <v>eWOODY_FUEL_ROTTEN_WOOD_LOADINGS_GREATER_THAN_THREE_INCHES_THREE_TO_NINE_INCHES</v>
       </c>
       <c r="B56" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="C56" s="5"/>
       <c r="D56" s="6"/>
       <c r="E56" s="41" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="F56" s="13">
         <v>5</v>
@@ -13126,12 +13126,12 @@
         <v>eWOODY_FUEL_ROTTEN_WOOD_LOADINGS_GREATER_THAN_THREE_INCHES_NINE_TO_TWENTY_INCHES</v>
       </c>
       <c r="B57" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="C57" s="5"/>
       <c r="D57" s="6"/>
       <c r="E57" s="41" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="F57" s="13">
         <v>11</v>
@@ -13221,12 +13221,12 @@
         <v>eWOODY_FUEL_ROTTEN_WOOD_LOADINGS_GREATER_THAN_THREE_INCHES_GREATER_THAN_TWENTY_INCHES</v>
       </c>
       <c r="B58" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="C58" s="5"/>
       <c r="D58" s="6"/>
       <c r="E58" s="41" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="F58" s="13">
         <v>0</v>
@@ -13316,7 +13316,7 @@
         <v>eWOODY_FUEL_STUMPS_SOUND_DIAMETER</v>
       </c>
       <c r="B59" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="C59" s="5"/>
       <c r="D59" s="6"/>
@@ -13406,7 +13406,7 @@
         <v>eWOODY_FUEL_STUMPS_SOUND_HEIGHT</v>
       </c>
       <c r="B60" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="C60" s="5"/>
       <c r="D60" s="6"/>
@@ -13496,7 +13496,7 @@
         <v>eWOODY_FUEL_STUMPS_SOUND_STEM_DENSITY</v>
       </c>
       <c r="B61" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="C61" s="5"/>
       <c r="D61" s="6"/>
@@ -13586,7 +13586,7 @@
         <v>eWOODY_FUEL_STUMPS_ROTTEN_DIAMETER</v>
       </c>
       <c r="B62" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="C62" s="5"/>
       <c r="D62" s="6"/>
@@ -13682,7 +13682,7 @@
         <v>eWOODY_FUEL_STUMPS_ROTTEN_HEIGHT</v>
       </c>
       <c r="B63" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="C63" s="5"/>
       <c r="D63" s="6"/>
@@ -13778,7 +13778,7 @@
         <v>eWOODY_FUEL_STUMPS_ROTTEN_STEM_DENSITY</v>
       </c>
       <c r="B64" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="C64" s="5"/>
       <c r="D64" s="6"/>
@@ -13874,7 +13874,7 @@
         <v>eWOODY_FUEL_STUMPS_LIGHTERED_PITCHY_DIAMETER</v>
       </c>
       <c r="B65" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="C65" s="5"/>
       <c r="D65" s="6"/>
@@ -13958,7 +13958,7 @@
         <v>eWOODY_FUEL_STUMPS_LIGHTERED_PITCHY_HEIGHT</v>
       </c>
       <c r="B66" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="C66" s="5"/>
       <c r="D66" s="6"/>
@@ -14042,7 +14042,7 @@
         <v>eWOODY_FUEL_STUMPS_LIGHTERED_PITCHY_STEM_DENSITY</v>
       </c>
       <c r="B67" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="C67" s="5"/>
       <c r="D67" s="6"/>
@@ -14126,7 +14126,7 @@
         <v>eWOODY_FUEL_PILES_CLEAN_LOADING</v>
       </c>
       <c r="B68" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="C68" s="5"/>
       <c r="D68" s="6"/>
@@ -14228,7 +14228,7 @@
         <v>eWOODY_FUEL_PILES_DIRTY_LOADING</v>
       </c>
       <c r="B69" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="C69" s="5"/>
       <c r="D69" s="6"/>
@@ -14330,7 +14330,7 @@
         <v>eWOODY_FUEL_PILES_VERYDIRTY_LOADING</v>
       </c>
       <c r="B70" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="C70" s="5"/>
       <c r="D70" s="6"/>
@@ -14432,7 +14432,7 @@
         <v>eLITTER_LITTER_TYPE_BROADLEAF_DECIDUOUS_RELATIVE_COVER</v>
       </c>
       <c r="B71" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="C71" s="5"/>
       <c r="D71" s="6"/>
@@ -14519,7 +14519,7 @@
         <v>eLITTER_LITTER_TYPE_BROADLEAF_EVERGREEN_RELATIVE_COVER</v>
       </c>
       <c r="B72" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="C72" s="5"/>
       <c r="D72" s="6"/>
@@ -14606,7 +14606,7 @@
         <v>eLITTER_LITTER_TYPE_GRASS_RELATIVE_COVER</v>
       </c>
       <c r="B73" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="C73" s="5"/>
       <c r="D73" s="6"/>
@@ -14693,7 +14693,7 @@
         <v>eLITTER_LITTER_TYPE_LONG_NEEDLE_PINE_RELATIVE_COVER</v>
       </c>
       <c r="B74" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="C74" s="5"/>
       <c r="D74" s="6"/>
@@ -14786,7 +14786,7 @@
         <v>eLITTER_LITTER_TYPE_OTHER_CONIFER_RELATIVE_COVER</v>
       </c>
       <c r="B75" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="C75" s="5"/>
       <c r="D75" s="6"/>
@@ -14876,7 +14876,7 @@
         <v>eLITTER_LITTER_TYPE_PALM_FROND_RELATIVE_COVER</v>
       </c>
       <c r="B76" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="C76" s="5"/>
       <c r="D76" s="6"/>
@@ -14963,7 +14963,7 @@
         <v>eLITTER_LITTER_TYPE_SHORT_NEEDLE_PINE_RELATIVE_COVER</v>
       </c>
       <c r="B77" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="C77" s="5"/>
       <c r="D77" s="6"/>
@@ -15047,7 +15047,7 @@
         <v>eMOSS_LICHEN_LITTER_GROUND_LICHEN_DEPTH</v>
       </c>
       <c r="B78" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="C78" s="5"/>
       <c r="D78" s="6"/>
@@ -15134,7 +15134,7 @@
         <v>eMOSS_LICHEN_LITTER_GROUND_LICHEN_PERCENT_COVER</v>
       </c>
       <c r="B79" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="C79" s="5"/>
       <c r="D79" s="6"/>
@@ -15221,7 +15221,7 @@
         <v>eMOSS_LICHEN_LITTER_LITTER_DEPTH</v>
       </c>
       <c r="B80" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="C80" s="5"/>
       <c r="D80" s="6">
@@ -15328,7 +15328,7 @@
         <v>eMOSS_LICHEN_LITTER_LITTER_PERCENT_COVER</v>
       </c>
       <c r="B81" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="C81" s="5"/>
       <c r="D81" s="6">
@@ -15435,7 +15435,7 @@
         <v>eMOSS_LICHEN_LITTER_MOSS_DEPTH</v>
       </c>
       <c r="B82" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="C82" s="5"/>
       <c r="D82" s="6"/>
@@ -15525,7 +15525,7 @@
         <v>eMOSS_LICHEN_LITTER_MOSS_PERCENT_COVER</v>
       </c>
       <c r="B83" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="C83" s="5"/>
       <c r="D83" s="6"/>
@@ -15615,7 +15615,7 @@
         <v>eGROUND_FUEL_DUFF_LOWER_DEPTH</v>
       </c>
       <c r="B84" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="C84" s="5"/>
       <c r="D84" s="6"/>
@@ -15705,7 +15705,7 @@
         <v>eGROUND_FUEL_DUFF_LOWER_PERCENT_COVER</v>
       </c>
       <c r="B85" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="C85" s="5"/>
       <c r="D85" s="6"/>
@@ -15795,7 +15795,7 @@
         <v>eGROUND_FUEL_DUFF_UPPER_DEPTH</v>
       </c>
       <c r="B86" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="C86" s="5"/>
       <c r="D86" s="6"/>
@@ -15897,7 +15897,7 @@
         <v>eGROUND_FUEL_DUFF_UPPER_PERCENT_COVER</v>
       </c>
       <c r="B87" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="C87" s="5"/>
       <c r="D87" s="6"/>
@@ -15999,7 +15999,7 @@
         <v>eGROUND_FUEL_BASAL_ACCUMULATION_DEPTH</v>
       </c>
       <c r="B88" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="C88" s="5"/>
       <c r="D88" s="6"/>
@@ -16083,7 +16083,7 @@
         <v>eGROUND_FUEL_BASAL_ACCUMULATION_NUMBER_PER_UNIT_AREA</v>
       </c>
       <c r="B89" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="C89" s="5"/>
       <c r="D89" s="6"/>
@@ -16167,7 +16167,7 @@
         <v>eGROUND_FUEL_BASAL_ACCUMULATION_RADIUS</v>
       </c>
       <c r="B90" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="C90" s="5"/>
       <c r="D90" s="6"/>
@@ -16251,7 +16251,7 @@
         <v>eGROUND_FUEL_SQUIRREL_MIDDENS_DEPTH</v>
       </c>
       <c r="B91" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="C91" s="5"/>
       <c r="D91" s="6"/>
@@ -16338,7 +16338,7 @@
         <v>eGROUND_FUEL_SQUIRREL_MIDDENS_NUMBER_PER_UNIT_AREA</v>
       </c>
       <c r="B92" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="C92" s="5"/>
       <c r="D92" s="6"/>
@@ -16425,7 +16425,7 @@
         <v>eGROUND_FUEL_SQUIRREL_MIDDENS_RADIUS</v>
       </c>
       <c r="B93" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="C93" s="5"/>
       <c r="D93" s="6"/>
@@ -16554,7 +16554,7 @@
         <v>33</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="C1" s="16" t="s">
         <v>215</v>
@@ -16644,7 +16644,7 @@
         <v>eCANOPY_TREES_TOTAL_PERCENT_COVER</v>
       </c>
       <c r="B2" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="C2" s="5">
         <v>0.6</v>
@@ -16744,7 +16744,7 @@
         <v>eCANOPY_TREES_OVERSTORY_DIAMETER_AT_BREAST_HEIGHT</v>
       </c>
       <c r="B3" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="C3" s="5"/>
       <c r="D3" s="9"/>
@@ -16840,7 +16840,7 @@
         <v>eCANOPY_TREES_OVERSTORY_HEIGHT_TO_LIVE_CROWN</v>
       </c>
       <c r="B4" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="C4" s="5">
         <v>1.2</v>
@@ -16938,7 +16938,7 @@
         <v>eCANOPY_TREES_OVERSTORY_HEIGHT</v>
       </c>
       <c r="B5" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="C5" s="5"/>
       <c r="D5" s="9"/>
@@ -17034,7 +17034,7 @@
         <v>eCANOPY_TREES_OVERSTORY_PERCENT_COVER</v>
       </c>
       <c r="B6" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="C6" s="5">
         <v>0.6</v>
@@ -17134,7 +17134,7 @@
         <v>eCANOPY_TREES_OVERSTORY_STEM_DENSITY</v>
       </c>
       <c r="B7" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="C7" s="5">
         <v>0.6</v>
@@ -17234,7 +17234,7 @@
         <v>eCANOPY_TREES_MIDSTORY_DIAMETER_AT_BREAST_HEIGHT</v>
       </c>
       <c r="B8" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="C8" s="5"/>
       <c r="D8" s="9"/>
@@ -17321,7 +17321,7 @@
         <v>eCANOPY_TREES_MIDSTORY_HEIGHT_TO_LIVE_CROWN</v>
       </c>
       <c r="B9" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="C9" s="5">
         <v>1.2</v>
@@ -17410,7 +17410,7 @@
         <v>eCANOPY_TREES_MIDSTORY_HEIGHT</v>
       </c>
       <c r="B10" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="C10" s="5"/>
       <c r="D10" s="9"/>
@@ -17497,7 +17497,7 @@
         <v>eCANOPY_TREES_MIDSTORY_PERCENT_COVER</v>
       </c>
       <c r="B11" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="C11" s="5">
         <v>0.6</v>
@@ -17588,7 +17588,7 @@
         <v>eCANOPY_TREES_MIDSTORY_STEM_DENSITY</v>
       </c>
       <c r="B12" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="C12" s="5">
         <v>0.6</v>
@@ -17679,7 +17679,7 @@
         <v>eCANOPY_TREES_UNDERSTORY_DIAMETER_AT_BREAST_HEIGHT</v>
       </c>
       <c r="B13" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="C13" s="5"/>
       <c r="D13" s="9"/>
@@ -17772,7 +17772,7 @@
         <v>eCANOPY_TREES_UNDERSTORY_HEIGHT_TO_LIVE_CROWN</v>
       </c>
       <c r="B14" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="C14" s="5"/>
       <c r="D14" s="9"/>
@@ -17865,7 +17865,7 @@
         <v>eCANOPY_TREES_UNDERSTORY_HEIGHT</v>
       </c>
       <c r="B15" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="C15" s="57"/>
       <c r="D15" s="9"/>
@@ -17958,7 +17958,7 @@
         <v>eCANOPY_TREES_UNDERSTORY_PERCENT_COVER</v>
       </c>
       <c r="B16" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="C16" s="5"/>
       <c r="D16" s="9"/>
@@ -18051,7 +18051,7 @@
         <v>eCANOPY_TREES_UNDERSTORY_STEM_DENSITY</v>
       </c>
       <c r="B17" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="C17" s="5"/>
       <c r="D17" s="9"/>
@@ -18144,14 +18144,14 @@
         <v>eCANOPY_SNAGS_CLASS_1_ALL_OTHERS_DIAMETER</v>
       </c>
       <c r="B18" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="C18" s="47"/>
       <c r="D18" s="49" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="E18" s="50" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="G18" s="14">
         <f t="shared" si="6"/>
@@ -18238,14 +18238,14 @@
         <v>eCANOPY_SNAGS_CLASS_1_ALL_OTHERS_HEIGHT</v>
       </c>
       <c r="B19" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="C19" s="47"/>
       <c r="D19" s="49" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="E19" s="50" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="G19" s="14">
         <f t="shared" si="6"/>
@@ -18332,14 +18332,14 @@
         <v>eCANOPY_SNAGS_CLASS_1_ALL_OTHERS_STEM_DENSITY</v>
       </c>
       <c r="B20" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="C20" s="47"/>
       <c r="D20" s="49" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="E20" s="50" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="G20" s="14">
         <f t="shared" si="6"/>
@@ -18426,13 +18426,13 @@
         <v>eCANOPY_SNAGS_CLASS_1_CONIFERS_WITH_FOLIAGE_HEIGHT_TO_CROWN_BASE</v>
       </c>
       <c r="B21" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="C21" s="48" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="D21" s="51" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="E21" s="41">
         <v>0</v>
@@ -18519,13 +18519,13 @@
         <v>eCANOPY_SNAGS_CLASS_1_CONIFERS_WITH_FOLIAGE_DIAMETER</v>
       </c>
       <c r="B22" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="C22" s="48" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="D22" s="51" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="E22" s="41">
         <v>0</v>
@@ -18612,13 +18612,13 @@
         <v>eCANOPY_SNAGS_CLASS_1_CONIFERS_WITH_FOLIAGE_HEIGHT</v>
       </c>
       <c r="B23" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="C23" s="48" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="D23" s="51" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="E23" s="41">
         <v>0</v>
@@ -18705,13 +18705,13 @@
         <v>eCANOPY_SNAGS_CLASS_1_CONIFERS_WITH_FOLIAGE_PERCENT_COVER</v>
       </c>
       <c r="B24" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="C24" s="52" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="D24" s="51" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="E24" s="41">
         <v>0</v>
@@ -18798,13 +18798,13 @@
         <v>eCANOPY_SNAGS_CLASS_1_CONIFERS_WITH_FOLIAGE_STEM_DENSITY</v>
       </c>
       <c r="B25" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="C25" s="48" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="D25" s="51" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="E25" s="41">
         <v>0</v>
@@ -18891,14 +18891,14 @@
         <v>eCANOPY_SNAGS_CLASS_2_DIAMETER</v>
       </c>
       <c r="B26" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="C26" s="47"/>
       <c r="D26" s="49" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="E26" s="50" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="G26" s="14">
         <f t="shared" ref="G26:I44" si="28">F26</f>
@@ -18988,14 +18988,14 @@
         <v>eCANOPY_SNAGS_CLASS_2_HEIGHT</v>
       </c>
       <c r="B27" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="C27" s="47"/>
       <c r="D27" s="49" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="E27" s="50" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="G27" s="14">
         <f t="shared" si="28"/>
@@ -19085,14 +19085,14 @@
         <v>eCANOPY_SNAGS_CLASS_2_STEM_DENSITY</v>
       </c>
       <c r="B28" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="C28" s="47"/>
       <c r="D28" s="49" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="E28" s="50" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="G28" s="14">
         <f t="shared" si="28"/>
@@ -19182,14 +19182,14 @@
         <v>eCANOPY_SNAGS_CLASS_3_DIAMETER</v>
       </c>
       <c r="B29" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="C29" s="47"/>
       <c r="D29" s="49" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="E29" s="50" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="F29" s="13">
         <v>9</v>
@@ -19282,14 +19282,14 @@
         <v>eCANOPY_SNAGS_CLASS_3_HEIGHT</v>
       </c>
       <c r="B30" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="C30" s="47"/>
       <c r="D30" s="49" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="E30" s="50" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="F30" s="13">
         <v>60</v>
@@ -19382,14 +19382,14 @@
         <v>eCANOPY_SNAGS_CLASS_3_STEM_DENSITY</v>
       </c>
       <c r="B31" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="C31" s="47"/>
       <c r="D31" s="49" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="E31" s="50" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="F31" s="13">
         <v>3</v>
@@ -19482,7 +19482,7 @@
         <v>eCANOPY_LADDER_FUELS_MAXIMUM_HEIGHT</v>
       </c>
       <c r="B32" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="C32" s="5"/>
       <c r="D32" s="9"/>
@@ -19572,7 +19572,7 @@
         <v>eCANOPY_LADDER_FUELS_MINIMUM_HEIGHT</v>
       </c>
       <c r="B33" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="C33" s="5"/>
       <c r="D33" s="9"/>
@@ -19662,7 +19662,7 @@
         <v>eSHRUBS_PRIMARY_LAYER_HEIGHT</v>
       </c>
       <c r="B34" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="C34" s="5"/>
       <c r="D34" s="9"/>
@@ -19764,7 +19764,7 @@
         <v>eSHRUBS_PRIMARY_LAYER_PERCENT_COVER</v>
       </c>
       <c r="B35" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="C35" s="5"/>
       <c r="D35" s="9"/>
@@ -19866,7 +19866,7 @@
         <v>eSHRUBS_PRIMARY_LAYER_PERCENT_LIVE</v>
       </c>
       <c r="B36" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="C36" s="5"/>
       <c r="D36" s="9"/>
@@ -19968,7 +19968,7 @@
         <v>eSHRUBS_SECONDARY_LAYER_HEIGHT</v>
       </c>
       <c r="B37" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="C37" s="5"/>
       <c r="D37" s="9"/>
@@ -20061,7 +20061,7 @@
         <v>eSHRUBS_SECONDARY_LAYER_PERCENT_COVER</v>
       </c>
       <c r="B38" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="C38" s="5"/>
       <c r="D38" s="9"/>
@@ -20154,7 +20154,7 @@
         <v>eSHRUBS_SECONDARY_LAYER_PERCENT_LIVE</v>
       </c>
       <c r="B39" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="C39" s="5"/>
       <c r="D39" s="9"/>
@@ -20247,7 +20247,7 @@
         <v>eHERBACEOUS_PRIMARY_LAYER_HEIGHT</v>
       </c>
       <c r="B40" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="C40" s="5"/>
       <c r="D40" s="9"/>
@@ -20346,7 +20346,7 @@
         <v>eHERBACEOUS_PRIMARY_LAYER_LOADING</v>
       </c>
       <c r="B41" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="C41" s="5"/>
       <c r="D41" s="9">
@@ -20447,7 +20447,7 @@
         <v>eHERBACEOUS_PRIMARY_LAYER_PERCENT_COVER</v>
       </c>
       <c r="B42" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="C42" s="5"/>
       <c r="D42" s="9">
@@ -20548,7 +20548,7 @@
         <v>eHERBACEOUS_PRIMARY_LAYER_PERCENT_LIVE</v>
       </c>
       <c r="B43" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="C43" s="5"/>
       <c r="D43" s="9"/>
@@ -20647,7 +20647,7 @@
         <v>eHERBACEOUS_SECONDARY_LAYER_HEIGHT</v>
       </c>
       <c r="B44" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C44" s="5"/>
       <c r="D44" s="9"/>
@@ -20743,7 +20743,7 @@
         <v>eHERBACEOUS_SECONDARY_LAYER_LOADING</v>
       </c>
       <c r="B45" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="C45" s="5"/>
       <c r="D45" s="9">
@@ -20841,7 +20841,7 @@
         <v>eHERBACEOUS_SECONDARY_LAYER_PERCENT_COVER</v>
       </c>
       <c r="B46" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="C46" s="5"/>
       <c r="D46" s="9">
@@ -20939,7 +20939,7 @@
         <v>eHERBACEOUS_SECONDARY_LAYER_PERCENT_LIVE</v>
       </c>
       <c r="B47" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="C47" s="5"/>
       <c r="D47" s="9"/>
@@ -21035,7 +21035,7 @@
         <v>eWOODY_FUEL_ALL_DOWNED_WOODY_FUEL_DEPTH</v>
       </c>
       <c r="B48" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="C48" s="5"/>
       <c r="D48" s="9">
@@ -21138,7 +21138,7 @@
         <v>eWOODY_FUEL_ALL_DOWNED_WOODY_FUEL_TOTAL_PERCENT_COVER</v>
       </c>
       <c r="B49" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="C49" s="5"/>
       <c r="D49" s="9">
@@ -21241,7 +21241,7 @@
         <v>eWOODY_FUEL_SOUND_WOOD_LOADINGS_ZERO_TO_THREE_INCHES_ONE_TO_THREE_INCHES</v>
       </c>
       <c r="B50" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="C50" s="5"/>
       <c r="D50" s="9">
@@ -21344,7 +21344,7 @@
         <v>eWOODY_FUEL_SOUND_WOOD_LOADINGS_ZERO_TO_THREE_INCHES_QUARTER_INCH_TO_ONE_INCH</v>
       </c>
       <c r="B51" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="C51" s="5"/>
       <c r="D51" s="9">
@@ -21447,7 +21447,7 @@
         <v>eWOODY_FUEL_SOUND_WOOD_LOADINGS_ZERO_TO_THREE_INCHES_ZERO_TO_QUARTER_INCH</v>
       </c>
       <c r="B52" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="C52" s="5"/>
       <c r="D52" s="9">
@@ -21550,7 +21550,7 @@
         <v>eWOODY_FUEL_SOUND_WOOD_LOADINGS_GREATER_THAN_THREE_INCHES_THREE_TO_NINE_INCHES</v>
       </c>
       <c r="B53" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="C53" s="5"/>
       <c r="D53" s="9"/>
@@ -21651,7 +21651,7 @@
         <v>eWOODY_FUEL_SOUND_WOOD_LOADINGS_GREATER_THAN_THREE_INCHES_NINE_TO_TWENTY_INCHES</v>
       </c>
       <c r="B54" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="C54" s="5"/>
       <c r="D54" s="9"/>
@@ -21752,7 +21752,7 @@
         <v>eWOODY_FUEL_SOUND_WOOD_LOADINGS_GREATER_THAN_THREE_INCHES_GREATER_THAN_TWENTY_INCHES</v>
       </c>
       <c r="B55" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="C55" s="5"/>
       <c r="D55" s="9"/>
@@ -21853,12 +21853,12 @@
         <v>eWOODY_FUEL_ROTTEN_WOOD_LOADINGS_GREATER_THAN_THREE_INCHES_THREE_TO_NINE_INCHES</v>
       </c>
       <c r="B56" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="C56" s="5"/>
       <c r="D56" s="9"/>
       <c r="E56" s="41" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="F56" s="13">
         <v>5</v>
@@ -21948,12 +21948,12 @@
         <v>eWOODY_FUEL_ROTTEN_WOOD_LOADINGS_GREATER_THAN_THREE_INCHES_NINE_TO_TWENTY_INCHES</v>
       </c>
       <c r="B57" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="C57" s="5"/>
       <c r="D57" s="9"/>
       <c r="E57" s="41" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="F57" s="13">
         <v>11</v>
@@ -22043,12 +22043,12 @@
         <v>eWOODY_FUEL_ROTTEN_WOOD_LOADINGS_GREATER_THAN_THREE_INCHES_GREATER_THAN_TWENTY_INCHES</v>
       </c>
       <c r="B58" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="C58" s="5"/>
       <c r="D58" s="9"/>
       <c r="E58" s="41" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="F58" s="13">
         <v>0</v>
@@ -22138,7 +22138,7 @@
         <v>eWOODY_FUEL_STUMPS_SOUND_DIAMETER</v>
       </c>
       <c r="B59" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="C59" s="5"/>
       <c r="D59" s="9"/>
@@ -22228,7 +22228,7 @@
         <v>eWOODY_FUEL_STUMPS_SOUND_HEIGHT</v>
       </c>
       <c r="B60" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="C60" s="5"/>
       <c r="D60" s="9"/>
@@ -22318,7 +22318,7 @@
         <v>eWOODY_FUEL_STUMPS_SOUND_STEM_DENSITY</v>
       </c>
       <c r="B61" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="C61" s="5"/>
       <c r="D61" s="9"/>
@@ -22408,7 +22408,7 @@
         <v>eWOODY_FUEL_STUMPS_ROTTEN_DIAMETER</v>
       </c>
       <c r="B62" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="C62" s="5"/>
       <c r="D62" s="9"/>
@@ -22504,7 +22504,7 @@
         <v>eWOODY_FUEL_STUMPS_ROTTEN_HEIGHT</v>
       </c>
       <c r="B63" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="C63" s="5"/>
       <c r="D63" s="9"/>
@@ -22600,7 +22600,7 @@
         <v>eWOODY_FUEL_STUMPS_ROTTEN_STEM_DENSITY</v>
       </c>
       <c r="B64" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="C64" s="5"/>
       <c r="D64" s="9"/>
@@ -22696,7 +22696,7 @@
         <v>eWOODY_FUEL_STUMPS_LIGHTERED_PITCHY_DIAMETER</v>
       </c>
       <c r="B65" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="C65" s="5"/>
       <c r="D65" s="9"/>
@@ -22780,7 +22780,7 @@
         <v>eWOODY_FUEL_STUMPS_LIGHTERED_PITCHY_HEIGHT</v>
       </c>
       <c r="B66" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="C66" s="5"/>
       <c r="D66" s="9"/>
@@ -22864,7 +22864,7 @@
         <v>eWOODY_FUEL_STUMPS_LIGHTERED_PITCHY_STEM_DENSITY</v>
       </c>
       <c r="B67" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="C67" s="5"/>
       <c r="D67" s="9"/>
@@ -22948,7 +22948,7 @@
         <v>eWOODY_FUEL_PILES_CLEAN_LOADING</v>
       </c>
       <c r="B68" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="C68" s="5"/>
       <c r="D68" s="9"/>
@@ -23050,7 +23050,7 @@
         <v>eWOODY_FUEL_PILES_DIRTY_LOADING</v>
       </c>
       <c r="B69" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="C69" s="5"/>
       <c r="D69" s="9"/>
@@ -23152,7 +23152,7 @@
         <v>eWOODY_FUEL_PILES_VERYDIRTY_LOADING</v>
       </c>
       <c r="B70" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="C70" s="5"/>
       <c r="D70" s="9"/>
@@ -23254,7 +23254,7 @@
         <v>eLITTER_LITTER_TYPE_BROADLEAF_DECIDUOUS_RELATIVE_COVER</v>
       </c>
       <c r="B71" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="C71" s="5"/>
       <c r="D71" s="9"/>
@@ -23341,7 +23341,7 @@
         <v>eLITTER_LITTER_TYPE_BROADLEAF_EVERGREEN_RELATIVE_COVER</v>
       </c>
       <c r="B72" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="C72" s="5"/>
       <c r="D72" s="9"/>
@@ -23428,7 +23428,7 @@
         <v>eLITTER_LITTER_TYPE_GRASS_RELATIVE_COVER</v>
       </c>
       <c r="B73" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="C73" s="5"/>
       <c r="D73" s="9"/>
@@ -23515,7 +23515,7 @@
         <v>eLITTER_LITTER_TYPE_LONG_NEEDLE_PINE_RELATIVE_COVER</v>
       </c>
       <c r="B74" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="C74" s="5"/>
       <c r="D74" s="9"/>
@@ -23608,7 +23608,7 @@
         <v>eLITTER_LITTER_TYPE_OTHER_CONIFER_RELATIVE_COVER</v>
       </c>
       <c r="B75" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="C75" s="5"/>
       <c r="D75" s="9"/>
@@ -23698,7 +23698,7 @@
         <v>eLITTER_LITTER_TYPE_PALM_FROND_RELATIVE_COVER</v>
       </c>
       <c r="B76" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="C76" s="5"/>
       <c r="D76" s="9"/>
@@ -23785,7 +23785,7 @@
         <v>eLITTER_LITTER_TYPE_SHORT_NEEDLE_PINE_RELATIVE_COVER</v>
       </c>
       <c r="B77" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="C77" s="5"/>
       <c r="D77" s="9"/>
@@ -23869,7 +23869,7 @@
         <v>eMOSS_LICHEN_LITTER_GROUND_LICHEN_DEPTH</v>
       </c>
       <c r="B78" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="C78" s="5"/>
       <c r="D78" s="9"/>
@@ -23956,7 +23956,7 @@
         <v>eMOSS_LICHEN_LITTER_GROUND_LICHEN_PERCENT_COVER</v>
       </c>
       <c r="B79" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="C79" s="5"/>
       <c r="D79" s="9"/>
@@ -24043,7 +24043,7 @@
         <v>eMOSS_LICHEN_LITTER_LITTER_DEPTH</v>
       </c>
       <c r="B80" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="C80" s="5"/>
       <c r="D80" s="9">
@@ -24150,7 +24150,7 @@
         <v>eMOSS_LICHEN_LITTER_LITTER_PERCENT_COVER</v>
       </c>
       <c r="B81" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="C81" s="5"/>
       <c r="D81" s="9">
@@ -24257,7 +24257,7 @@
         <v>eMOSS_LICHEN_LITTER_MOSS_DEPTH</v>
       </c>
       <c r="B82" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="C82" s="5"/>
       <c r="D82" s="9"/>
@@ -24347,7 +24347,7 @@
         <v>eMOSS_LICHEN_LITTER_MOSS_PERCENT_COVER</v>
       </c>
       <c r="B83" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="C83" s="5"/>
       <c r="D83" s="9"/>
@@ -24437,7 +24437,7 @@
         <v>eGROUND_FUEL_DUFF_LOWER_DEPTH</v>
       </c>
       <c r="B84" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="C84" s="5"/>
       <c r="D84" s="9"/>
@@ -24527,7 +24527,7 @@
         <v>eGROUND_FUEL_DUFF_LOWER_PERCENT_COVER</v>
       </c>
       <c r="B85" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="C85" s="5"/>
       <c r="D85" s="9"/>
@@ -24617,7 +24617,7 @@
         <v>eGROUND_FUEL_DUFF_UPPER_DEPTH</v>
       </c>
       <c r="B86" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="C86" s="5"/>
       <c r="D86" s="9"/>
@@ -24721,7 +24721,7 @@
         <v>eGROUND_FUEL_DUFF_UPPER_PERCENT_COVER</v>
       </c>
       <c r="B87" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="C87" s="5"/>
       <c r="D87" s="9"/>
@@ -24825,7 +24825,7 @@
         <v>eGROUND_FUEL_BASAL_ACCUMULATION_DEPTH</v>
       </c>
       <c r="B88" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="C88" s="5"/>
       <c r="D88" s="9"/>
@@ -24909,7 +24909,7 @@
         <v>eGROUND_FUEL_BASAL_ACCUMULATION_NUMBER_PER_UNIT_AREA</v>
       </c>
       <c r="B89" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="C89" s="5"/>
       <c r="D89" s="9"/>
@@ -24993,7 +24993,7 @@
         <v>eGROUND_FUEL_BASAL_ACCUMULATION_RADIUS</v>
       </c>
       <c r="B90" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="C90" s="5"/>
       <c r="D90" s="9"/>
@@ -25077,7 +25077,7 @@
         <v>eGROUND_FUEL_SQUIRREL_MIDDENS_DEPTH</v>
       </c>
       <c r="B91" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="C91" s="5"/>
       <c r="D91" s="9"/>
@@ -25164,7 +25164,7 @@
         <v>eGROUND_FUEL_SQUIRREL_MIDDENS_NUMBER_PER_UNIT_AREA</v>
       </c>
       <c r="B92" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="C92" s="5"/>
       <c r="D92" s="9"/>
@@ -25251,7 +25251,7 @@
         <v>eGROUND_FUEL_SQUIRREL_MIDDENS_RADIUS</v>
       </c>
       <c r="B93" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="C93" s="5"/>
       <c r="D93" s="9"/>
@@ -25397,7 +25397,7 @@
         <v>33</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="C2" s="16" t="s">
         <v>219</v>
@@ -25487,7 +25487,7 @@
         <v>eCANOPY_TREES_TOTAL_PERCENT_COVER</v>
       </c>
       <c r="B3" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="C3" s="5">
         <v>0.25</v>
@@ -25587,7 +25587,7 @@
         <v>eCANOPY_TREES_OVERSTORY_DIAMETER_AT_BREAST_HEIGHT</v>
       </c>
       <c r="B4" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="C4" s="5"/>
       <c r="D4" s="6"/>
@@ -25683,7 +25683,7 @@
         <v>eCANOPY_TREES_OVERSTORY_HEIGHT_TO_LIVE_CROWN</v>
       </c>
       <c r="B5" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="C5" s="5">
         <v>1.3</v>
@@ -25781,7 +25781,7 @@
         <v>eCANOPY_TREES_OVERSTORY_HEIGHT</v>
       </c>
       <c r="B6" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="6"/>
@@ -25877,7 +25877,7 @@
         <v>eCANOPY_TREES_OVERSTORY_PERCENT_COVER</v>
       </c>
       <c r="B7" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="C7" s="5">
         <v>0.25</v>
@@ -25977,7 +25977,7 @@
         <v>eCANOPY_TREES_OVERSTORY_STEM_DENSITY</v>
       </c>
       <c r="B8" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="C8" s="5">
         <v>0.25</v>
@@ -26077,7 +26077,7 @@
         <v>eCANOPY_TREES_MIDSTORY_DIAMETER_AT_BREAST_HEIGHT</v>
       </c>
       <c r="B9" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="C9" s="5"/>
       <c r="D9" s="6"/>
@@ -26164,7 +26164,7 @@
         <v>eCANOPY_TREES_MIDSTORY_HEIGHT_TO_LIVE_CROWN</v>
       </c>
       <c r="B10" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="C10" s="5">
         <v>1.3</v>
@@ -26253,7 +26253,7 @@
         <v>eCANOPY_TREES_MIDSTORY_HEIGHT</v>
       </c>
       <c r="B11" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="C11" s="5"/>
       <c r="D11" s="6"/>
@@ -26340,7 +26340,7 @@
         <v>eCANOPY_TREES_MIDSTORY_PERCENT_COVER</v>
       </c>
       <c r="B12" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="C12" s="5">
         <v>0.25</v>
@@ -26431,7 +26431,7 @@
         <v>eCANOPY_TREES_MIDSTORY_STEM_DENSITY</v>
       </c>
       <c r="B13" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="C13" s="5">
         <v>0.25</v>
@@ -26522,7 +26522,7 @@
         <v>eCANOPY_TREES_UNDERSTORY_DIAMETER_AT_BREAST_HEIGHT</v>
       </c>
       <c r="B14" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="C14" s="5"/>
       <c r="D14" s="6"/>
@@ -26615,7 +26615,7 @@
         <v>eCANOPY_TREES_UNDERSTORY_HEIGHT_TO_LIVE_CROWN</v>
       </c>
       <c r="B15" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="C15" s="5"/>
       <c r="D15" s="6"/>
@@ -26708,7 +26708,7 @@
         <v>eCANOPY_TREES_UNDERSTORY_HEIGHT</v>
       </c>
       <c r="B16" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="C16" s="5"/>
       <c r="D16" s="6"/>
@@ -26801,7 +26801,7 @@
         <v>eCANOPY_TREES_UNDERSTORY_PERCENT_COVER</v>
       </c>
       <c r="B17" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="C17" s="5"/>
       <c r="D17" s="6"/>
@@ -26894,7 +26894,7 @@
         <v>eCANOPY_TREES_UNDERSTORY_STEM_DENSITY</v>
       </c>
       <c r="B18" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="C18" s="5"/>
       <c r="D18" s="6"/>
@@ -26987,14 +26987,14 @@
         <v>eCANOPY_SNAGS_CLASS_1_ALL_OTHERS_DIAMETER</v>
       </c>
       <c r="B19" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="C19" s="47"/>
       <c r="D19" s="49" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="E19" s="50" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="G19" s="14">
         <f t="shared" si="16"/>
@@ -27081,14 +27081,14 @@
         <v>eCANOPY_SNAGS_CLASS_1_ALL_OTHERS_HEIGHT</v>
       </c>
       <c r="B20" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="C20" s="47"/>
       <c r="D20" s="49" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="E20" s="50" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="G20" s="14">
         <f t="shared" si="16"/>
@@ -27175,14 +27175,14 @@
         <v>eCANOPY_SNAGS_CLASS_1_ALL_OTHERS_STEM_DENSITY</v>
       </c>
       <c r="B21" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="C21" s="53"/>
       <c r="D21" s="49" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="E21" s="50" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="G21" s="14">
         <f t="shared" si="16"/>
@@ -27269,13 +27269,13 @@
         <v>eCANOPY_SNAGS_CLASS_1_CONIFERS_WITH_FOLIAGE_HEIGHT_TO_CROWN_BASE</v>
       </c>
       <c r="B22" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="C22" s="55" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="D22" s="51" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="E22" s="42">
         <v>0</v>
@@ -27362,13 +27362,13 @@
         <v>eCANOPY_SNAGS_CLASS_1_CONIFERS_WITH_FOLIAGE_DIAMETER</v>
       </c>
       <c r="B23" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="C23" s="55" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="D23" s="51" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="E23" s="42">
         <v>0</v>
@@ -27455,13 +27455,13 @@
         <v>eCANOPY_SNAGS_CLASS_1_CONIFERS_WITH_FOLIAGE_HEIGHT</v>
       </c>
       <c r="B24" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="C24" s="55" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="D24" s="51" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="E24" s="42">
         <v>0</v>
@@ -27548,13 +27548,13 @@
         <v>eCANOPY_SNAGS_CLASS_1_CONIFERS_WITH_FOLIAGE_PERCENT_COVER</v>
       </c>
       <c r="B25" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="C25" s="56" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="D25" s="51" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="E25" s="42">
         <v>0</v>
@@ -27641,13 +27641,13 @@
         <v>eCANOPY_SNAGS_CLASS_1_CONIFERS_WITH_FOLIAGE_STEM_DENSITY</v>
       </c>
       <c r="B26" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="C26" s="55" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="D26" s="51" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="E26" s="42">
         <v>0</v>
@@ -27734,14 +27734,14 @@
         <v>eCANOPY_SNAGS_CLASS_2_DIAMETER</v>
       </c>
       <c r="B27" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="C27" s="54"/>
       <c r="D27" s="49" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="E27" s="50" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="G27" s="14">
         <f>F27</f>
@@ -27831,14 +27831,14 @@
         <v>eCANOPY_SNAGS_CLASS_2_HEIGHT</v>
       </c>
       <c r="B28" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="C28" s="47"/>
       <c r="D28" s="49" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="E28" s="50" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="G28" s="14">
         <f>F28</f>
@@ -27928,14 +27928,14 @@
         <v>eCANOPY_SNAGS_CLASS_2_STEM_DENSITY</v>
       </c>
       <c r="B29" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="C29" s="47"/>
       <c r="D29" s="49" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="E29" s="50" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="G29" s="14">
         <f t="shared" ref="G29:I92" si="38">F29</f>
@@ -28025,14 +28025,14 @@
         <v>eCANOPY_SNAGS_CLASS_3_DIAMETER</v>
       </c>
       <c r="B30" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="C30" s="47"/>
       <c r="D30" s="49" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="E30" s="50" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="F30" s="13">
         <v>9</v>
@@ -28125,14 +28125,14 @@
         <v>eCANOPY_SNAGS_CLASS_3_HEIGHT</v>
       </c>
       <c r="B31" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="C31" s="47"/>
       <c r="D31" s="49" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="E31" s="50" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="F31" s="13">
         <v>60</v>
@@ -28225,14 +28225,14 @@
         <v>eCANOPY_SNAGS_CLASS_3_STEM_DENSITY</v>
       </c>
       <c r="B32" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="C32" s="47"/>
       <c r="D32" s="49" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="E32" s="50" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="F32" s="13">
         <v>3</v>
@@ -28325,7 +28325,7 @@
         <v>eCANOPY_LADDER_FUELS_MAXIMUM_HEIGHT</v>
       </c>
       <c r="B33" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="C33" s="5"/>
       <c r="D33" s="6"/>
@@ -28415,7 +28415,7 @@
         <v>eCANOPY_LADDER_FUELS_MINIMUM_HEIGHT</v>
       </c>
       <c r="B34" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="C34" s="5"/>
       <c r="D34" s="6"/>
@@ -28505,7 +28505,7 @@
         <v>eSHRUBS_PRIMARY_LAYER_HEIGHT</v>
       </c>
       <c r="B35" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="C35" s="5"/>
       <c r="D35" s="9"/>
@@ -28607,7 +28607,7 @@
         <v>eSHRUBS_PRIMARY_LAYER_PERCENT_COVER</v>
       </c>
       <c r="B36" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="C36" s="5"/>
       <c r="D36" s="9">
@@ -28711,7 +28711,7 @@
         <v>eSHRUBS_PRIMARY_LAYER_PERCENT_LIVE</v>
       </c>
       <c r="B37" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="C37" s="5"/>
       <c r="D37" s="9"/>
@@ -28813,7 +28813,7 @@
         <v>eSHRUBS_SECONDARY_LAYER_HEIGHT</v>
       </c>
       <c r="B38" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="C38" s="5"/>
       <c r="D38" s="9"/>
@@ -28906,7 +28906,7 @@
         <v>eSHRUBS_SECONDARY_LAYER_PERCENT_COVER</v>
       </c>
       <c r="B39" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="C39" s="5"/>
       <c r="D39" s="9">
@@ -29001,7 +29001,7 @@
         <v>eSHRUBS_SECONDARY_LAYER_PERCENT_LIVE</v>
       </c>
       <c r="B40" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="C40" s="5"/>
       <c r="D40" s="9"/>
@@ -29094,7 +29094,7 @@
         <v>eHERBACEOUS_PRIMARY_LAYER_HEIGHT</v>
       </c>
       <c r="B41" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="C41" s="5"/>
       <c r="D41" s="9"/>
@@ -29193,7 +29193,7 @@
         <v>eHERBACEOUS_PRIMARY_LAYER_LOADING</v>
       </c>
       <c r="B42" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="C42" s="5"/>
       <c r="D42" s="9">
@@ -29294,7 +29294,7 @@
         <v>eHERBACEOUS_PRIMARY_LAYER_PERCENT_COVER</v>
       </c>
       <c r="B43" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="C43" s="5"/>
       <c r="D43" s="9">
@@ -29395,7 +29395,7 @@
         <v>eHERBACEOUS_PRIMARY_LAYER_PERCENT_LIVE</v>
       </c>
       <c r="B44" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="C44" s="5"/>
       <c r="D44" s="9"/>
@@ -29494,7 +29494,7 @@
         <v>eHERBACEOUS_SECONDARY_LAYER_HEIGHT</v>
       </c>
       <c r="B45" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C45" s="5"/>
       <c r="D45" s="9"/>
@@ -29590,7 +29590,7 @@
         <v>eHERBACEOUS_SECONDARY_LAYER_LOADING</v>
       </c>
       <c r="B46" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="C46" s="5"/>
       <c r="D46" s="9">
@@ -29688,7 +29688,7 @@
         <v>eHERBACEOUS_SECONDARY_LAYER_PERCENT_COVER</v>
       </c>
       <c r="B47" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="C47" s="5"/>
       <c r="D47" s="9">
@@ -29786,7 +29786,7 @@
         <v>eHERBACEOUS_SECONDARY_LAYER_PERCENT_LIVE</v>
       </c>
       <c r="B48" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="C48" s="5"/>
       <c r="D48" s="9"/>
@@ -29882,7 +29882,7 @@
         <v>eWOODY_FUEL_ALL_DOWNED_WOODY_FUEL_DEPTH</v>
       </c>
       <c r="B49" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="C49" s="5"/>
       <c r="D49" s="9">
@@ -29983,7 +29983,7 @@
         <v>eWOODY_FUEL_ALL_DOWNED_WOODY_FUEL_TOTAL_PERCENT_COVER</v>
       </c>
       <c r="B50" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="C50" s="5"/>
       <c r="D50" s="9">
@@ -30084,7 +30084,7 @@
         <v>eWOODY_FUEL_SOUND_WOOD_LOADINGS_ZERO_TO_THREE_INCHES_ONE_TO_THREE_INCHES</v>
       </c>
       <c r="B51" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="C51" s="5"/>
       <c r="D51" s="9">
@@ -30187,7 +30187,7 @@
         <v>eWOODY_FUEL_SOUND_WOOD_LOADINGS_ZERO_TO_THREE_INCHES_QUARTER_INCH_TO_ONE_INCH</v>
       </c>
       <c r="B52" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="C52" s="5"/>
       <c r="D52" s="9">
@@ -30290,7 +30290,7 @@
         <v>eWOODY_FUEL_SOUND_WOOD_LOADINGS_ZERO_TO_THREE_INCHES_ZERO_TO_QUARTER_INCH</v>
       </c>
       <c r="B53" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="C53" s="5"/>
       <c r="D53" s="9">
@@ -30393,7 +30393,7 @@
         <v>eWOODY_FUEL_SOUND_WOOD_LOADINGS_GREATER_THAN_THREE_INCHES_THREE_TO_NINE_INCHES</v>
       </c>
       <c r="B54" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="C54" s="5"/>
       <c r="D54" s="6"/>
@@ -30494,7 +30494,7 @@
         <v>eWOODY_FUEL_SOUND_WOOD_LOADINGS_GREATER_THAN_THREE_INCHES_NINE_TO_TWENTY_INCHES</v>
       </c>
       <c r="B55" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="C55" s="5"/>
       <c r="D55" s="6"/>
@@ -30595,7 +30595,7 @@
         <v>eWOODY_FUEL_SOUND_WOOD_LOADINGS_GREATER_THAN_THREE_INCHES_GREATER_THAN_TWENTY_INCHES</v>
       </c>
       <c r="B56" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="C56" s="5"/>
       <c r="D56" s="6"/>
@@ -30696,12 +30696,12 @@
         <v>eWOODY_FUEL_ROTTEN_WOOD_LOADINGS_GREATER_THAN_THREE_INCHES_THREE_TO_NINE_INCHES</v>
       </c>
       <c r="B57" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="C57" s="5"/>
       <c r="D57" s="6"/>
       <c r="E57" s="41" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="F57" s="13">
         <v>5</v>
@@ -30791,12 +30791,12 @@
         <v>eWOODY_FUEL_ROTTEN_WOOD_LOADINGS_GREATER_THAN_THREE_INCHES_NINE_TO_TWENTY_INCHES</v>
       </c>
       <c r="B58" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="C58" s="5"/>
       <c r="D58" s="6"/>
       <c r="E58" s="41" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="F58" s="13">
         <v>11</v>
@@ -30886,12 +30886,12 @@
         <v>eWOODY_FUEL_ROTTEN_WOOD_LOADINGS_GREATER_THAN_THREE_INCHES_GREATER_THAN_TWENTY_INCHES</v>
       </c>
       <c r="B59" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="C59" s="5"/>
       <c r="D59" s="6"/>
       <c r="E59" s="41" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="F59" s="13">
         <v>0</v>
@@ -30981,7 +30981,7 @@
         <v>eWOODY_FUEL_STUMPS_SOUND_DIAMETER</v>
       </c>
       <c r="B60" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="C60" s="5"/>
       <c r="D60" s="6"/>
@@ -31071,7 +31071,7 @@
         <v>eWOODY_FUEL_STUMPS_SOUND_HEIGHT</v>
       </c>
       <c r="B61" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="C61" s="5"/>
       <c r="D61" s="6"/>
@@ -31161,7 +31161,7 @@
         <v>eWOODY_FUEL_STUMPS_SOUND_STEM_DENSITY</v>
       </c>
       <c r="B62" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="C62" s="5"/>
       <c r="D62" s="6"/>
@@ -31251,7 +31251,7 @@
         <v>eWOODY_FUEL_STUMPS_ROTTEN_DIAMETER</v>
       </c>
       <c r="B63" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="C63" s="5"/>
       <c r="D63" s="6"/>
@@ -31347,7 +31347,7 @@
         <v>eWOODY_FUEL_STUMPS_ROTTEN_HEIGHT</v>
       </c>
       <c r="B64" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="C64" s="5"/>
       <c r="D64" s="6"/>
@@ -31443,7 +31443,7 @@
         <v>eWOODY_FUEL_STUMPS_ROTTEN_STEM_DENSITY</v>
       </c>
       <c r="B65" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="C65" s="5"/>
       <c r="D65" s="6"/>
@@ -31539,7 +31539,7 @@
         <v>eWOODY_FUEL_STUMPS_LIGHTERED_PITCHY_DIAMETER</v>
       </c>
       <c r="B66" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="C66" s="5"/>
       <c r="D66" s="6"/>
@@ -31623,7 +31623,7 @@
         <v>eWOODY_FUEL_STUMPS_LIGHTERED_PITCHY_HEIGHT</v>
       </c>
       <c r="B67" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="C67" s="5"/>
       <c r="D67" s="6"/>
@@ -31707,7 +31707,7 @@
         <v>eWOODY_FUEL_STUMPS_LIGHTERED_PITCHY_STEM_DENSITY</v>
       </c>
       <c r="B68" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="C68" s="5"/>
       <c r="D68" s="6"/>
@@ -31791,7 +31791,7 @@
         <v>eWOODY_FUEL_PILES_CLEAN_LOADING</v>
       </c>
       <c r="B69" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="C69" s="5"/>
       <c r="D69" s="6"/>
@@ -31893,7 +31893,7 @@
         <v>eWOODY_FUEL_PILES_DIRTY_LOADING</v>
       </c>
       <c r="B70" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="C70" s="5"/>
       <c r="D70" s="6"/>
@@ -31995,7 +31995,7 @@
         <v>eWOODY_FUEL_PILES_VERYDIRTY_LOADING</v>
       </c>
       <c r="B71" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="C71" s="5"/>
       <c r="D71" s="6"/>
@@ -32097,7 +32097,7 @@
         <v>eLITTER_LITTER_TYPE_BROADLEAF_DECIDUOUS_RELATIVE_COVER</v>
       </c>
       <c r="B72" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="C72" s="5"/>
       <c r="D72" s="6"/>
@@ -32184,7 +32184,7 @@
         <v>eLITTER_LITTER_TYPE_BROADLEAF_EVERGREEN_RELATIVE_COVER</v>
       </c>
       <c r="B73" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="C73" s="5"/>
       <c r="D73" s="6"/>
@@ -32271,7 +32271,7 @@
         <v>eLITTER_LITTER_TYPE_GRASS_RELATIVE_COVER</v>
       </c>
       <c r="B74" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="C74" s="5"/>
       <c r="D74" s="6"/>
@@ -32358,7 +32358,7 @@
         <v>eLITTER_LITTER_TYPE_LONG_NEEDLE_PINE_RELATIVE_COVER</v>
       </c>
       <c r="B75" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="C75" s="5"/>
       <c r="D75" s="6"/>
@@ -32451,7 +32451,7 @@
         <v>eLITTER_LITTER_TYPE_OTHER_CONIFER_RELATIVE_COVER</v>
       </c>
       <c r="B76" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="C76" s="5"/>
       <c r="D76" s="6"/>
@@ -32541,7 +32541,7 @@
         <v>eLITTER_LITTER_TYPE_PALM_FROND_RELATIVE_COVER</v>
       </c>
       <c r="B77" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="C77" s="5"/>
       <c r="D77" s="6"/>
@@ -32628,7 +32628,7 @@
         <v>eLITTER_LITTER_TYPE_SHORT_NEEDLE_PINE_RELATIVE_COVER</v>
       </c>
       <c r="B78" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="C78" s="5"/>
       <c r="D78" s="6"/>
@@ -32712,7 +32712,7 @@
         <v>eMOSS_LICHEN_LITTER_GROUND_LICHEN_DEPTH</v>
       </c>
       <c r="B79" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="C79" s="5"/>
       <c r="D79" s="9"/>
@@ -32799,7 +32799,7 @@
         <v>eMOSS_LICHEN_LITTER_GROUND_LICHEN_PERCENT_COVER</v>
       </c>
       <c r="B80" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="C80" s="5"/>
       <c r="D80" s="9"/>
@@ -32886,7 +32886,7 @@
         <v>eMOSS_LICHEN_LITTER_LITTER_DEPTH</v>
       </c>
       <c r="B81" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="C81" s="5"/>
       <c r="D81" s="9">
@@ -32992,7 +32992,7 @@
         <v>eMOSS_LICHEN_LITTER_LITTER_PERCENT_COVER</v>
       </c>
       <c r="B82" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="C82" s="5"/>
       <c r="D82" s="9">
@@ -33098,7 +33098,7 @@
         <v>eMOSS_LICHEN_LITTER_MOSS_DEPTH</v>
       </c>
       <c r="B83" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="C83" s="5"/>
       <c r="D83" s="9"/>
@@ -33188,7 +33188,7 @@
         <v>eMOSS_LICHEN_LITTER_MOSS_PERCENT_COVER</v>
       </c>
       <c r="B84" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="C84" s="5"/>
       <c r="D84" s="9"/>
@@ -33278,7 +33278,7 @@
         <v>eGROUND_FUEL_DUFF_LOWER_DEPTH</v>
       </c>
       <c r="B85" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="C85" s="5"/>
       <c r="D85" s="6"/>
@@ -33368,7 +33368,7 @@
         <v>eGROUND_FUEL_DUFF_LOWER_PERCENT_COVER</v>
       </c>
       <c r="B86" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="C86" s="5"/>
       <c r="D86" s="6"/>
@@ -33458,7 +33458,7 @@
         <v>eGROUND_FUEL_DUFF_UPPER_DEPTH</v>
       </c>
       <c r="B87" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="C87" s="5"/>
       <c r="D87" s="6"/>
@@ -33562,7 +33562,7 @@
         <v>eGROUND_FUEL_DUFF_UPPER_PERCENT_COVER</v>
       </c>
       <c r="B88" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="C88" s="5"/>
       <c r="D88" s="6"/>
@@ -33666,7 +33666,7 @@
         <v>eGROUND_FUEL_BASAL_ACCUMULATION_DEPTH</v>
       </c>
       <c r="B89" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="C89" s="5"/>
       <c r="D89" s="6"/>
@@ -33750,7 +33750,7 @@
         <v>eGROUND_FUEL_BASAL_ACCUMULATION_NUMBER_PER_UNIT_AREA</v>
       </c>
       <c r="B90" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="C90" s="5"/>
       <c r="D90" s="6"/>
@@ -33834,7 +33834,7 @@
         <v>eGROUND_FUEL_BASAL_ACCUMULATION_RADIUS</v>
       </c>
       <c r="B91" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="C91" s="5"/>
       <c r="D91" s="6"/>
@@ -33918,7 +33918,7 @@
         <v>eGROUND_FUEL_SQUIRREL_MIDDENS_DEPTH</v>
       </c>
       <c r="B92" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="C92" s="5"/>
       <c r="D92" s="6"/>
@@ -34005,7 +34005,7 @@
         <v>eGROUND_FUEL_SQUIRREL_MIDDENS_NUMBER_PER_UNIT_AREA</v>
       </c>
       <c r="B93" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="C93" s="5"/>
       <c r="D93" s="6"/>
@@ -34092,7 +34092,7 @@
         <v>eGROUND_FUEL_SQUIRREL_MIDDENS_RADIUS</v>
       </c>
       <c r="B94" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="C94" s="5"/>
       <c r="D94" s="6"/>
@@ -34212,181 +34212,181 @@
         <v>19</v>
       </c>
       <c r="C1" t="s">
+        <v>230</v>
+      </c>
+      <c r="D1" t="s">
+        <v>231</v>
+      </c>
+      <c r="E1" t="s">
         <v>232</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>233</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>234</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>235</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>236</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>237</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>238</v>
-      </c>
-      <c r="J1" t="s">
-        <v>239</v>
-      </c>
-      <c r="K1" t="s">
-        <v>240</v>
       </c>
       <c r="L1" t="s">
         <v>20</v>
       </c>
       <c r="M1" t="s">
+        <v>239</v>
+      </c>
+      <c r="N1" t="s">
+        <v>240</v>
+      </c>
+      <c r="O1" t="s">
         <v>241</v>
       </c>
-      <c r="N1" t="s">
+      <c r="P1" t="s">
         <v>242</v>
       </c>
-      <c r="O1" t="s">
+      <c r="Q1" t="s">
         <v>243</v>
       </c>
-      <c r="P1" t="s">
+      <c r="R1" t="s">
         <v>244</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="S1" t="s">
         <v>245</v>
       </c>
-      <c r="R1" t="s">
+      <c r="T1" t="s">
         <v>246</v>
       </c>
-      <c r="S1" t="s">
+      <c r="U1" t="s">
         <v>247</v>
-      </c>
-      <c r="T1" t="s">
-        <v>248</v>
-      </c>
-      <c r="U1" t="s">
-        <v>249</v>
       </c>
       <c r="V1" t="s">
         <v>21</v>
       </c>
       <c r="W1" t="s">
+        <v>248</v>
+      </c>
+      <c r="X1" t="s">
+        <v>249</v>
+      </c>
+      <c r="Y1" t="s">
         <v>250</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Z1" t="s">
         <v>251</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="AA1" t="s">
         <v>252</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AB1" t="s">
         <v>253</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AC1" t="s">
         <v>254</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AD1" t="s">
         <v>255</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AE1" t="s">
         <v>256</v>
-      </c>
-      <c r="AD1" t="s">
-        <v>257</v>
-      </c>
-      <c r="AE1" t="s">
-        <v>258</v>
       </c>
       <c r="AF1" t="s">
         <v>26</v>
       </c>
       <c r="AG1" t="s">
+        <v>257</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>258</v>
+      </c>
+      <c r="AI1" t="s">
         <v>259</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AJ1" t="s">
         <v>260</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AK1" t="s">
         <v>261</v>
       </c>
-      <c r="AJ1" t="s">
+      <c r="AL1" t="s">
         <v>262</v>
       </c>
-      <c r="AK1" t="s">
+      <c r="AM1" t="s">
         <v>263</v>
       </c>
-      <c r="AL1" t="s">
+      <c r="AN1" t="s">
         <v>264</v>
       </c>
-      <c r="AM1" t="s">
+      <c r="AO1" t="s">
         <v>265</v>
-      </c>
-      <c r="AN1" t="s">
-        <v>266</v>
-      </c>
-      <c r="AO1" t="s">
-        <v>267</v>
       </c>
       <c r="AP1" t="s">
         <v>27</v>
       </c>
       <c r="AQ1" t="s">
+        <v>266</v>
+      </c>
+      <c r="AR1" t="s">
+        <v>267</v>
+      </c>
+      <c r="AS1" t="s">
         <v>268</v>
       </c>
-      <c r="AR1" t="s">
+      <c r="AT1" t="s">
         <v>269</v>
       </c>
-      <c r="AS1" t="s">
+      <c r="AU1" t="s">
         <v>270</v>
       </c>
-      <c r="AT1" t="s">
+      <c r="AV1" t="s">
         <v>271</v>
       </c>
-      <c r="AU1" t="s">
+      <c r="AW1" t="s">
         <v>272</v>
       </c>
-      <c r="AV1" t="s">
+      <c r="AX1" t="s">
         <v>273</v>
       </c>
-      <c r="AW1" t="s">
+      <c r="AY1" t="s">
         <v>274</v>
-      </c>
-      <c r="AX1" t="s">
-        <v>275</v>
-      </c>
-      <c r="AY1" t="s">
-        <v>276</v>
       </c>
       <c r="AZ1" t="s">
         <v>32</v>
       </c>
       <c r="BA1" t="s">
+        <v>275</v>
+      </c>
+      <c r="BB1" t="s">
+        <v>276</v>
+      </c>
+      <c r="BC1" t="s">
         <v>277</v>
       </c>
-      <c r="BB1" t="s">
+      <c r="BD1" t="s">
         <v>278</v>
       </c>
-      <c r="BC1" t="s">
+      <c r="BE1" t="s">
         <v>279</v>
       </c>
-      <c r="BD1" t="s">
+      <c r="BF1" t="s">
         <v>280</v>
       </c>
-      <c r="BE1" t="s">
+      <c r="BG1" t="s">
         <v>281</v>
       </c>
-      <c r="BF1" t="s">
+      <c r="BH1" t="s">
         <v>282</v>
       </c>
-      <c r="BG1" t="s">
+      <c r="BI1" t="s">
         <v>283</v>
-      </c>
-      <c r="BH1" t="s">
-        <v>284</v>
-      </c>
-      <c r="BI1" t="s">
-        <v>285</v>
       </c>
     </row>
     <row r="2" spans="1:61" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Corrected Insects low severity expected values
</commit_message>
<xml_diff>
--- a/specifications/5_Insects/ScriptRules_Insects.xlsx
+++ b/specifications/5_Insects/ScriptRules_Insects.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13380" windowHeight="10260" firstSheet="3" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13380" windowHeight="10260" firstSheet="3" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="FBDescriptions" sheetId="9" r:id="rId1"/>
@@ -7709,8 +7709,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AC93"/>
   <sheetViews>
-    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+    <sheetView tabSelected="1" topLeftCell="L1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="AC2" sqref="AC2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8146,11 +8146,11 @@
         <v>100</v>
       </c>
       <c r="K5" s="12">
-        <f t="shared" ref="K5" si="14">J5</f>
+        <f t="shared" ref="K5:K17" si="14">J5</f>
         <v>0</v>
       </c>
       <c r="L5" s="15">
-        <f t="shared" ref="L5" si="15">K5</f>
+        <f t="shared" ref="L5:L17" si="15">K5</f>
         <v>0</v>
       </c>
       <c r="M5" s="16">
@@ -8158,11 +8158,11 @@
         <v>0</v>
       </c>
       <c r="O5" s="12">
-        <f t="shared" ref="O5" si="16">N5</f>
+        <f t="shared" ref="O5:O17" si="16">N5</f>
         <v>0</v>
       </c>
       <c r="P5" s="15">
-        <f t="shared" ref="P5" si="17">O5</f>
+        <f t="shared" ref="P5:P17" si="17">O5</f>
         <v>0</v>
       </c>
       <c r="Q5" s="16">
@@ -8173,11 +8173,11 @@
         <v>25</v>
       </c>
       <c r="S5" s="12">
-        <f t="shared" ref="S5" si="18">R5</f>
+        <f t="shared" ref="S5:S17" si="18">R5</f>
         <v>25</v>
       </c>
       <c r="T5" s="15">
-        <f t="shared" ref="T5" si="19">S5</f>
+        <f t="shared" ref="T5:T17" si="19">S5</f>
         <v>25</v>
       </c>
       <c r="U5" s="16">
@@ -8188,11 +8188,11 @@
         <v>60</v>
       </c>
       <c r="W5" s="12">
-        <f t="shared" ref="W5" si="20">V5</f>
+        <f t="shared" ref="W5:W17" si="20">V5</f>
         <v>60</v>
       </c>
       <c r="X5" s="15">
-        <f t="shared" ref="X5" si="21">W5</f>
+        <f t="shared" ref="X5:X17" si="21">W5</f>
         <v>60</v>
       </c>
       <c r="Y5" s="16">
@@ -8203,11 +8203,11 @@
         <v>78</v>
       </c>
       <c r="AA5" s="12">
-        <f t="shared" ref="AA5" si="22">Z5</f>
+        <f t="shared" ref="AA5:AA17" si="22">Z5</f>
         <v>78</v>
       </c>
       <c r="AB5" s="15">
-        <f t="shared" ref="AB5" si="23">AA5</f>
+        <f t="shared" ref="AB5:AB17" si="23">AA5</f>
         <v>78</v>
       </c>
       <c r="AC5" s="16">
@@ -8439,11 +8439,11 @@
         <v>0</v>
       </c>
       <c r="K8" s="12">
-        <f t="shared" ref="K8" si="24">J8</f>
+        <f t="shared" ref="K8:K20" si="24">J8</f>
         <v>0</v>
       </c>
       <c r="L8" s="15">
-        <f t="shared" ref="L8" si="25">K8</f>
+        <f t="shared" ref="L8:L20" si="25">K8</f>
         <v>0</v>
       </c>
       <c r="M8" s="16">
@@ -8451,11 +8451,11 @@
         <v>0</v>
       </c>
       <c r="O8" s="12">
-        <f t="shared" ref="O8" si="26">N8</f>
+        <f t="shared" ref="O8:O20" si="26">N8</f>
         <v>0</v>
       </c>
       <c r="P8" s="15">
-        <f t="shared" ref="P8" si="27">O8</f>
+        <f t="shared" ref="P8:P20" si="27">O8</f>
         <v>0</v>
       </c>
       <c r="Q8" s="16">
@@ -8463,11 +8463,11 @@
         <v>0</v>
       </c>
       <c r="S8" s="12">
-        <f t="shared" ref="S8" si="28">R8</f>
+        <f t="shared" ref="S8:S20" si="28">R8</f>
         <v>0</v>
       </c>
       <c r="T8" s="15">
-        <f t="shared" ref="T8" si="29">S8</f>
+        <f t="shared" ref="T8:T20" si="29">S8</f>
         <v>0</v>
       </c>
       <c r="U8" s="16">
@@ -8478,11 +8478,11 @@
         <v>7.5</v>
       </c>
       <c r="W8" s="12">
-        <f t="shared" ref="W8" si="30">V8</f>
+        <f t="shared" ref="W8:W20" si="30">V8</f>
         <v>7.5</v>
       </c>
       <c r="X8" s="15">
-        <f t="shared" ref="X8" si="31">W8</f>
+        <f t="shared" ref="X8:X20" si="31">W8</f>
         <v>7.5</v>
       </c>
       <c r="Y8" s="16">
@@ -8490,11 +8490,11 @@
         <v>7.5</v>
       </c>
       <c r="AA8" s="12">
-        <f t="shared" ref="AA8" si="32">Z8</f>
+        <f t="shared" ref="AA8:AA20" si="32">Z8</f>
         <v>0</v>
       </c>
       <c r="AB8" s="15">
-        <f t="shared" ref="AB8" si="33">AA8</f>
+        <f t="shared" ref="AB8:AB20" si="33">AA8</f>
         <v>0</v>
       </c>
       <c r="AC8" s="16">
@@ -8617,11 +8617,11 @@
         <v>0</v>
       </c>
       <c r="K10" s="12">
-        <f t="shared" ref="K10" si="34">J10</f>
+        <f t="shared" ref="K10:K22" si="34">J10</f>
         <v>0</v>
       </c>
       <c r="L10" s="15">
-        <f t="shared" ref="L10" si="35">K10</f>
+        <f t="shared" ref="L10:L22" si="35">K10</f>
         <v>0</v>
       </c>
       <c r="M10" s="16">
@@ -8629,11 +8629,11 @@
         <v>0</v>
       </c>
       <c r="O10" s="12">
-        <f t="shared" ref="O10" si="36">N10</f>
+        <f t="shared" ref="O10:O22" si="36">N10</f>
         <v>0</v>
       </c>
       <c r="P10" s="15">
-        <f t="shared" ref="P10" si="37">O10</f>
+        <f t="shared" ref="P10:P22" si="37">O10</f>
         <v>0</v>
       </c>
       <c r="Q10" s="16">
@@ -8641,11 +8641,11 @@
         <v>0</v>
       </c>
       <c r="S10" s="12">
-        <f t="shared" ref="S10" si="38">R10</f>
+        <f t="shared" ref="S10:S22" si="38">R10</f>
         <v>0</v>
       </c>
       <c r="T10" s="15">
-        <f t="shared" ref="T10" si="39">S10</f>
+        <f t="shared" ref="T10:T22" si="39">S10</f>
         <v>0</v>
       </c>
       <c r="U10" s="16">
@@ -8656,11 +8656,11 @@
         <v>44</v>
       </c>
       <c r="W10" s="12">
-        <f t="shared" ref="W10" si="40">V10</f>
+        <f t="shared" ref="W10:W22" si="40">V10</f>
         <v>44</v>
       </c>
       <c r="X10" s="15">
-        <f t="shared" ref="X10" si="41">W10</f>
+        <f t="shared" ref="X10:X22" si="41">W10</f>
         <v>44</v>
       </c>
       <c r="Y10" s="16">
@@ -8668,11 +8668,11 @@
         <v>44</v>
       </c>
       <c r="AA10" s="12">
-        <f t="shared" ref="AA10" si="42">Z10</f>
+        <f t="shared" ref="AA10:AA22" si="42">Z10</f>
         <v>0</v>
       </c>
       <c r="AB10" s="15">
-        <f t="shared" ref="AB10" si="43">AA10</f>
+        <f t="shared" ref="AB10:AB22" si="43">AA10</f>
         <v>0</v>
       </c>
       <c r="AC10" s="16">
@@ -8886,11 +8886,11 @@
         <v>0</v>
       </c>
       <c r="K13" s="12">
-        <f t="shared" ref="K13:K17" si="44">J13</f>
+        <f t="shared" ref="K13:K25" si="44">J13</f>
         <v>0</v>
       </c>
       <c r="L13" s="15">
-        <f t="shared" ref="L13:L17" si="45">K13</f>
+        <f t="shared" ref="L13:L25" si="45">K13</f>
         <v>0</v>
       </c>
       <c r="M13" s="16">
@@ -8898,11 +8898,11 @@
         <v>0</v>
       </c>
       <c r="O13" s="12">
-        <f t="shared" ref="O13:O17" si="46">N13</f>
+        <f t="shared" ref="O13:O25" si="46">N13</f>
         <v>0</v>
       </c>
       <c r="P13" s="15">
-        <f t="shared" ref="P13:P17" si="47">O13</f>
+        <f t="shared" ref="P13:P25" si="47">O13</f>
         <v>0</v>
       </c>
       <c r="Q13" s="16">
@@ -8913,11 +8913,11 @@
         <v>0.5</v>
       </c>
       <c r="S13" s="12">
-        <f t="shared" ref="S13:S17" si="48">R13</f>
+        <f t="shared" ref="S13:S25" si="48">R13</f>
         <v>0.5</v>
       </c>
       <c r="T13" s="15">
-        <f t="shared" ref="T13:T17" si="49">S13</f>
+        <f t="shared" ref="T13:T25" si="49">S13</f>
         <v>0.5</v>
       </c>
       <c r="U13" s="16">
@@ -8928,11 +8928,11 @@
         <v>1.7</v>
       </c>
       <c r="W13" s="12">
-        <f t="shared" ref="W13:W17" si="50">V13</f>
+        <f t="shared" ref="W13:W25" si="50">V13</f>
         <v>1.7</v>
       </c>
       <c r="X13" s="15">
-        <f t="shared" ref="X13:X17" si="51">W13</f>
+        <f t="shared" ref="X13:X25" si="51">W13</f>
         <v>1.7</v>
       </c>
       <c r="Y13" s="16">
@@ -8943,11 +8943,11 @@
         <v>1</v>
       </c>
       <c r="AA13" s="12">
-        <f t="shared" ref="AA13:AA17" si="52">Z13</f>
+        <f t="shared" ref="AA13:AA25" si="52">Z13</f>
         <v>1</v>
       </c>
       <c r="AB13" s="15">
-        <f t="shared" ref="AB13:AB17" si="53">AA13</f>
+        <f t="shared" ref="AB13:AB25" si="53">AA13</f>
         <v>1</v>
       </c>
       <c r="AC13" s="16">
@@ -9590,7 +9590,7 @@
       </c>
       <c r="X20" s="15">
         <f>W25</f>
-        <v>19.5</v>
+        <v>24.5</v>
       </c>
       <c r="Y20" s="20">
         <f>X24</f>
@@ -9918,11 +9918,11 @@
         <v>0</v>
       </c>
       <c r="K24" s="12">
-        <f>J24+J2*0.1</f>
+        <f>J24+(J2*0.1)</f>
         <v>0</v>
       </c>
       <c r="L24" s="15">
-        <f>K24+K2*0.05</f>
+        <f>K24+(K2*0.05)</f>
         <v>0</v>
       </c>
       <c r="M24" s="16">
@@ -9930,11 +9930,11 @@
         <v>0</v>
       </c>
       <c r="O24" s="12">
-        <f>N24+N2*0.1</f>
+        <f>N24+(N2*0.1)</f>
         <v>0</v>
       </c>
       <c r="P24" s="15">
-        <f>O24+O2*0.05</f>
+        <f>O24+(O2*0.05)</f>
         <v>0</v>
       </c>
       <c r="Q24" s="16">
@@ -9942,11 +9942,11 @@
         <v>0</v>
       </c>
       <c r="S24" s="12">
-        <f>R24+R2*0.1</f>
+        <f>R24+(R2*0.1)</f>
         <v>8</v>
       </c>
       <c r="T24" s="15">
-        <f>S24+S2*0.05</f>
+        <f>S24+(S2*0.05)</f>
         <v>11.6</v>
       </c>
       <c r="U24" s="16">
@@ -9957,11 +9957,11 @@
         <v>0.5071</v>
       </c>
       <c r="W24" s="12">
-        <f>V24+V2*0.1</f>
+        <f>V24+(V2*0.1)</f>
         <v>9.0070999999999994</v>
       </c>
       <c r="X24" s="15">
-        <f>W24+W2*0.05</f>
+        <f>W24+(W2*0.05)</f>
         <v>12.832100000000001</v>
       </c>
       <c r="Y24" s="16">
@@ -9969,11 +9969,11 @@
         <v>0</v>
       </c>
       <c r="AA24" s="12">
-        <f>Z24+Z2*0.1</f>
+        <f>Z24+(Z2*0.1)</f>
         <v>6</v>
       </c>
       <c r="AB24" s="15">
-        <f>AA24+AA2*0.05</f>
+        <f>AA24+(AA2*0.05)</f>
         <v>8.6999999999999993</v>
       </c>
       <c r="AC24" s="16">
@@ -9999,23 +9999,23 @@
         <v>0</v>
       </c>
       <c r="G25" s="12">
-        <f>(0.1*F7)+(0.1*F12)</f>
+        <f>F25+(0.1*F7)+(0.1*F12)</f>
         <v>1.2000000000000002</v>
       </c>
       <c r="H25" s="15">
-        <f>(0.05*G7)+(0.05*G12)</f>
-        <v>0.54</v>
+        <f>G25+(0.05*G7)+(0.05*G12)</f>
+        <v>1.7400000000000002</v>
       </c>
       <c r="I25" s="16">
         <f>H25*$E25</f>
         <v>0</v>
       </c>
       <c r="K25" s="12">
-        <f>(0.1*J7)+(0.1*J12)</f>
+        <f>J25+(0.1*J7)+(0.1*J12)</f>
         <v>0</v>
       </c>
       <c r="L25" s="15">
-        <f>(0.05*K7)+(0.05*K12)</f>
+        <f>K25+(0.05*K7)+(0.05*K12)</f>
         <v>0</v>
       </c>
       <c r="M25" s="16">
@@ -10023,11 +10023,11 @@
         <v>0</v>
       </c>
       <c r="O25" s="12">
-        <f>(0.1*N7)+(0.1*N12)</f>
+        <f>N25+(0.1*N7)+(0.1*N12)</f>
         <v>0</v>
       </c>
       <c r="P25" s="15">
-        <f>(0.05*O7)+(0.05*O12)</f>
+        <f>O25+(0.05*O7)+(0.05*O12)</f>
         <v>0</v>
       </c>
       <c r="Q25" s="16">
@@ -10035,12 +10035,12 @@
         <v>0</v>
       </c>
       <c r="S25" s="12">
-        <f>(0.1*R7)+(0.1*R12)</f>
+        <f>R25+(0.1*R7)+(0.1*R12)</f>
         <v>350</v>
       </c>
       <c r="T25" s="15">
-        <f>(0.05*S7)+(0.05*S12)</f>
-        <v>157.5</v>
+        <f>S25+(0.05*S7)+(0.05*S12)</f>
+        <v>507.5</v>
       </c>
       <c r="U25" s="16">
         <f>T25*$E25</f>
@@ -10050,24 +10050,24 @@
         <v>5</v>
       </c>
       <c r="W25" s="12">
-        <f>(0.1*V7)+(0.1*V12)</f>
-        <v>19.5</v>
+        <f>V25+(0.1*V7)+(0.1*V12)</f>
+        <v>24.5</v>
       </c>
       <c r="X25" s="15">
-        <f>(0.05*W7)+(0.05*W12)</f>
-        <v>8.7750000000000004</v>
+        <f>W25+(0.05*W7)+(0.05*W12)</f>
+        <v>33.274999999999999</v>
       </c>
       <c r="Y25" s="16">
         <f>X25*$E25</f>
         <v>0</v>
       </c>
       <c r="AA25" s="12">
-        <f>(0.1*Z7)+(0.1*Z12)</f>
+        <f>Z25+(0.1*Z7)+(0.1*Z12)</f>
         <v>10</v>
       </c>
       <c r="AB25" s="15">
-        <f>(0.05*AA7)+(0.05*AA12)</f>
-        <v>4.5</v>
+        <f>AA25+(0.05*AA7)+(0.05*AA12)</f>
+        <v>14.5</v>
       </c>
       <c r="AC25" s="16">
         <f>AB25*$E25</f>
@@ -10347,7 +10347,7 @@
       </c>
       <c r="Y28" s="16">
         <f t="shared" si="67"/>
-        <v>19.5</v>
+        <v>24.5</v>
       </c>
       <c r="Z28" s="11">
         <v>3</v>
@@ -12761,7 +12761,7 @@
         <v>0</v>
       </c>
       <c r="L53" s="15">
-        <f t="shared" ref="L53:L79" si="106">K53</f>
+        <f t="shared" ref="L53:L93" si="106">K53</f>
         <v>0</v>
       </c>
       <c r="M53" s="16">
@@ -12773,7 +12773,7 @@
         <v>0</v>
       </c>
       <c r="P53" s="15">
-        <f t="shared" ref="P53:P79" si="107">O53</f>
+        <f t="shared" ref="P53:P93" si="107">O53</f>
         <v>0</v>
       </c>
       <c r="Q53" s="16">
@@ -12788,7 +12788,7 @@
         <v>1</v>
       </c>
       <c r="T53" s="15">
-        <f t="shared" ref="T53:T79" si="108">S53</f>
+        <f t="shared" ref="T53:T93" si="108">S53</f>
         <v>1</v>
       </c>
       <c r="U53" s="16">
@@ -12803,7 +12803,7 @@
         <v>1.2</v>
       </c>
       <c r="X53" s="15">
-        <f t="shared" ref="X53:X79" si="109">W53</f>
+        <f t="shared" ref="X53:X93" si="109">W53</f>
         <v>1.2</v>
       </c>
       <c r="Y53" s="16">
@@ -12818,7 +12818,7 @@
         <v>0.5</v>
       </c>
       <c r="AB53" s="15">
-        <f t="shared" ref="AB53:AB79" si="110">AA53</f>
+        <f t="shared" ref="AB53:AB93" si="110">AA53</f>
         <v>0.5</v>
       </c>
       <c r="AC53" s="16">
@@ -13348,7 +13348,7 @@
         <v>0</v>
       </c>
       <c r="M59" s="16">
-        <f t="shared" ref="M59:M79" si="112">L56</f>
+        <f t="shared" ref="M59:M93" si="112">L56</f>
         <v>0</v>
       </c>
       <c r="O59" s="12">
@@ -13360,7 +13360,7 @@
         <v>0</v>
       </c>
       <c r="Q59" s="16">
-        <f t="shared" ref="Q59:Q79" si="113">P56</f>
+        <f t="shared" ref="Q59:Q93" si="113">P56</f>
         <v>0</v>
       </c>
       <c r="R59" s="11">
@@ -13375,7 +13375,7 @@
         <v>3.5</v>
       </c>
       <c r="U59" s="16">
-        <f t="shared" ref="U59:U79" si="114">T56</f>
+        <f t="shared" ref="U59:U93" si="114">T56</f>
         <v>0.5</v>
       </c>
       <c r="W59" s="12">
@@ -13387,7 +13387,7 @@
         <v>0</v>
       </c>
       <c r="Y59" s="16">
-        <f t="shared" ref="Y59:Y79" si="115">X56</f>
+        <f t="shared" ref="Y59:Y93" si="115">X56</f>
         <v>0.75</v>
       </c>
       <c r="AA59" s="12">
@@ -13399,7 +13399,7 @@
         <v>0</v>
       </c>
       <c r="AC59" s="16">
-        <f t="shared" ref="AC59:AC79" si="116">AB56</f>
+        <f t="shared" ref="AC59:AC93" si="116">AB56</f>
         <v>0</v>
       </c>
     </row>
@@ -16520,7 +16520,7 @@
   <dimension ref="A1:AC93"/>
   <sheetViews>
     <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -25349,8 +25349,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AC93"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -38980,7 +38980,7 @@
       </c>
       <c r="AR20">
         <f>'51_Insects_LowSeverity'!X20</f>
-        <v>19.5</v>
+        <v>24.5</v>
       </c>
       <c r="AS20">
         <f>'51_Insects_LowSeverity'!Y20</f>
@@ -40050,7 +40050,7 @@
       </c>
       <c r="D25">
         <f>'51_Insects_LowSeverity'!H25</f>
-        <v>0.54</v>
+        <v>1.7400000000000002</v>
       </c>
       <c r="E25">
         <f>'51_Insects_LowSeverity'!I25</f>
@@ -40170,7 +40170,7 @@
       </c>
       <c r="AH25">
         <f>'51_Insects_LowSeverity'!T25</f>
-        <v>157.5</v>
+        <v>507.5</v>
       </c>
       <c r="AI25">
         <f>'51_Insects_LowSeverity'!U25</f>
@@ -40206,11 +40206,11 @@
       </c>
       <c r="AQ25">
         <f>'51_Insects_LowSeverity'!W25</f>
-        <v>19.5</v>
+        <v>24.5</v>
       </c>
       <c r="AR25">
         <f>'51_Insects_LowSeverity'!X25</f>
-        <v>8.7750000000000004</v>
+        <v>33.274999999999999</v>
       </c>
       <c r="AS25">
         <f>'51_Insects_LowSeverity'!Y25</f>
@@ -40250,7 +40250,7 @@
       </c>
       <c r="BB25">
         <f>'51_Insects_LowSeverity'!AB25</f>
-        <v>4.5</v>
+        <v>14.5</v>
       </c>
       <c r="BC25">
         <f>'51_Insects_LowSeverity'!AC25</f>
@@ -40952,7 +40952,7 @@
       </c>
       <c r="AS28">
         <f>'51_Insects_LowSeverity'!Y28</f>
-        <v>19.5</v>
+        <v>24.5</v>
       </c>
       <c r="AT28">
         <f>'52_Insects_ModSeverity'!W28</f>

</xml_diff>